<commit_message>
Modificacion de actividades Lunes 13 de febrero
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MATEO\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MATEO\Desktop\Platzi\Curso Git - GutHub\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34B65EF0-8179-456C-9370-339E2A3249CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{202A588B-B73A-40D4-BF99-684A8BFD0A6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{A899F46E-BA08-4AC6-A7C3-F03724044CD5}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="86">
   <si>
     <t>Hora</t>
   </si>
@@ -288,6 +288,12 @@
   </si>
   <si>
     <t>Cena - Guardar Ropa</t>
+  </si>
+  <si>
+    <t>Proyecto de redes 1</t>
+  </si>
+  <si>
+    <t>Practica 1 Analogica 2</t>
   </si>
 </sst>
 </file>
@@ -463,10 +469,16 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -487,16 +499,10 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -505,10 +511,10 @@
     <xf numFmtId="0" fontId="3" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -827,8 +833,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9132D586-DE4C-4B7E-830E-683E06A9C036}">
   <dimension ref="A2:R55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F52" sqref="F52"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13:C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1078,19 +1084,19 @@
       <c r="A9" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="C9" s="11" t="s">
+      <c r="B9" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="C9" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="D9" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="E9" s="11" t="s">
+      <c r="D9" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="F9" s="19" t="s">
+      <c r="F9" s="11" t="s">
         <v>33</v>
       </c>
       <c r="G9" s="23"/>
@@ -1100,19 +1106,19 @@
       <c r="K9" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="L9" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="M9" s="11" t="s">
+      <c r="L9" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="M9" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="N9" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="O9" s="11" t="s">
+      <c r="N9" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="O9" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="P9" s="19" t="s">
+      <c r="P9" s="11" t="s">
         <v>33</v>
       </c>
       <c r="Q9" s="23"/>
@@ -1122,11 +1128,11 @@
       <c r="A10" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="22"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="22"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="22"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="12"/>
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
       <c r="I10" s="1"/>
@@ -1134,11 +1140,11 @@
       <c r="K10" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="L10" s="22"/>
-      <c r="M10" s="11"/>
-      <c r="N10" s="22"/>
-      <c r="O10" s="11"/>
-      <c r="P10" s="22"/>
+      <c r="L10" s="12"/>
+      <c r="M10" s="14"/>
+      <c r="N10" s="12"/>
+      <c r="O10" s="14"/>
+      <c r="P10" s="12"/>
       <c r="Q10" s="5"/>
       <c r="R10" s="5"/>
     </row>
@@ -1146,25 +1152,25 @@
       <c r="A11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="D11" s="11" t="s">
+      <c r="D11" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="E11" s="11" t="s">
+      <c r="E11" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="F11" s="11" t="s">
+      <c r="F11" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="G11" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="H11" s="19" t="s">
+      <c r="G11" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="H11" s="11" t="s">
         <v>33</v>
       </c>
       <c r="I11" s="1"/>
@@ -1172,25 +1178,25 @@
       <c r="K11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L11" s="11" t="s">
+      <c r="L11" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="M11" s="11" t="s">
+      <c r="M11" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="N11" s="11" t="s">
+      <c r="N11" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="O11" s="11" t="s">
+      <c r="O11" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="P11" s="11" t="s">
+      <c r="P11" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="Q11" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="R11" s="19" t="s">
+      <c r="Q11" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="R11" s="11" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1198,47 +1204,47 @@
       <c r="A12" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="11"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="19"/>
-      <c r="H12" s="19"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
       <c r="K12" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="L12" s="11"/>
-      <c r="M12" s="11"/>
-      <c r="N12" s="11"/>
-      <c r="O12" s="11"/>
-      <c r="P12" s="11"/>
-      <c r="Q12" s="19"/>
-      <c r="R12" s="19"/>
+      <c r="L12" s="14"/>
+      <c r="M12" s="14"/>
+      <c r="N12" s="14"/>
+      <c r="O12" s="14"/>
+      <c r="P12" s="14"/>
+      <c r="Q12" s="11"/>
+      <c r="R12" s="11"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C13" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="C13" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="D13" s="11" t="s">
+      <c r="D13" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="E13" s="11" t="s">
+      <c r="E13" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="F13" s="11" t="s">
+      <c r="F13" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="G13" s="19"/>
-      <c r="H13" s="19"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
       <c r="K13" s="3" t="s">
@@ -1247,20 +1253,20 @@
       <c r="L13" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="M13" s="11" t="s">
+      <c r="M13" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="N13" s="11" t="s">
+      <c r="N13" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="O13" s="11" t="s">
+      <c r="O13" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="P13" s="11" t="s">
+      <c r="P13" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="Q13" s="19"/>
-      <c r="R13" s="19"/>
+      <c r="Q13" s="11"/>
+      <c r="R13" s="11"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
@@ -1269,12 +1275,12 @@
       <c r="B14" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="19"/>
-      <c r="H14" s="19"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
       <c r="K14" s="3" t="s">
@@ -1283,12 +1289,12 @@
       <c r="L14" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="M14" s="11"/>
-      <c r="N14" s="11"/>
-      <c r="O14" s="11"/>
-      <c r="P14" s="11"/>
-      <c r="Q14" s="19"/>
-      <c r="R14" s="19"/>
+      <c r="M14" s="14"/>
+      <c r="N14" s="14"/>
+      <c r="O14" s="14"/>
+      <c r="P14" s="14"/>
+      <c r="Q14" s="11"/>
+      <c r="R14" s="11"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
@@ -1346,25 +1352,25 @@
       <c r="A16" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="C16" s="19" t="s">
+      <c r="B16" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="11" t="s">
         <v>33</v>
       </c>
       <c r="D16" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="E16" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="F16" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="G16" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="H16" s="16" t="s">
+      <c r="E16" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="G16" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="H16" s="18" t="s">
         <v>33</v>
       </c>
       <c r="I16" s="1"/>
@@ -1372,25 +1378,25 @@
       <c r="K16" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="L16" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="M16" s="19" t="s">
+      <c r="L16" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="M16" s="11" t="s">
         <v>33</v>
       </c>
       <c r="N16" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="O16" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="P16" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q16" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="R16" s="16" t="s">
+      <c r="O16" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="P16" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q16" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="R16" s="18" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1398,105 +1404,105 @@
       <c r="A17" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="19"/>
-      <c r="C17" s="19"/>
-      <c r="D17" s="11" t="s">
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="E17" s="19"/>
-      <c r="F17" s="19"/>
-      <c r="G17" s="17"/>
-      <c r="H17" s="17"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="19"/>
+      <c r="H17" s="19"/>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
       <c r="K17" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="L17" s="19"/>
-      <c r="M17" s="19"/>
-      <c r="N17" s="11" t="s">
+      <c r="L17" s="11"/>
+      <c r="M17" s="11"/>
+      <c r="N17" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="O17" s="19"/>
-      <c r="P17" s="19"/>
-      <c r="Q17" s="17"/>
-      <c r="R17" s="17"/>
+      <c r="O17" s="11"/>
+      <c r="P17" s="11"/>
+      <c r="Q17" s="19"/>
+      <c r="R17" s="19"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="11" t="s">
+      <c r="B18" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="C18" s="11" t="s">
+      <c r="C18" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="D18" s="11"/>
-      <c r="E18" s="19"/>
-      <c r="F18" s="11" t="s">
+      <c r="D18" s="14"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="G18" s="17"/>
-      <c r="H18" s="17"/>
+      <c r="G18" s="19"/>
+      <c r="H18" s="19"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
       <c r="K18" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="L18" s="11" t="s">
+      <c r="L18" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="M18" s="11" t="s">
+      <c r="M18" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="N18" s="11"/>
-      <c r="O18" s="19"/>
-      <c r="P18" s="11" t="s">
+      <c r="N18" s="14"/>
+      <c r="O18" s="11"/>
+      <c r="P18" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="Q18" s="17"/>
-      <c r="R18" s="17"/>
+      <c r="Q18" s="19"/>
+      <c r="R18" s="19"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="11"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="E19" s="19"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="17"/>
-      <c r="H19" s="18"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E19" s="11"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="19"/>
+      <c r="H19" s="20"/>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
       <c r="K19" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="L19" s="11"/>
-      <c r="M19" s="11"/>
-      <c r="N19" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="O19" s="19"/>
-      <c r="P19" s="11"/>
-      <c r="Q19" s="17"/>
-      <c r="R19" s="18"/>
+      <c r="L19" s="14"/>
+      <c r="M19" s="14"/>
+      <c r="N19" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="O19" s="11"/>
+      <c r="P19" s="14"/>
+      <c r="Q19" s="19"/>
+      <c r="R19" s="20"/>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="11"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="19"/>
-      <c r="E20" s="19"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="18"/>
-      <c r="H20" s="20" t="s">
+      <c r="B20" s="14"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="20"/>
+      <c r="H20" s="21" t="s">
         <v>53</v>
       </c>
       <c r="I20" s="1"/>
@@ -1504,13 +1510,13 @@
       <c r="K20" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="L20" s="11"/>
-      <c r="M20" s="11"/>
-      <c r="N20" s="19"/>
-      <c r="O20" s="19"/>
-      <c r="P20" s="11"/>
-      <c r="Q20" s="18"/>
-      <c r="R20" s="20" t="s">
+      <c r="L20" s="14"/>
+      <c r="M20" s="14"/>
+      <c r="N20" s="11"/>
+      <c r="O20" s="11"/>
+      <c r="P20" s="14"/>
+      <c r="Q20" s="20"/>
+      <c r="R20" s="21" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1518,59 +1524,59 @@
       <c r="A21" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B21" s="12" t="s">
+      <c r="B21" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="C21" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="D21" s="12" t="s">
+      <c r="C21" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D21" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="E21" s="11" t="s">
+      <c r="E21" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="F21" s="12" t="s">
+      <c r="F21" s="13" t="s">
         <v>43</v>
       </c>
       <c r="G21" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="H21" s="21"/>
+      <c r="H21" s="22"/>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
       <c r="K21" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="L21" s="12" t="s">
+      <c r="L21" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="M21" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="N21" s="12" t="s">
+      <c r="M21" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="N21" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="O21" s="11" t="s">
+      <c r="O21" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="P21" s="12" t="s">
+      <c r="P21" s="13" t="s">
         <v>43</v>
       </c>
       <c r="Q21" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="R21" s="21"/>
+      <c r="R21" s="22"/>
     </row>
     <row r="22" spans="1:18" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B22" s="12"/>
-      <c r="C22" s="22"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="12"/>
+      <c r="B22" s="13"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="13"/>
       <c r="G22" s="8" t="s">
         <v>36</v>
       </c>
@@ -1582,11 +1588,11 @@
       <c r="K22" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="L22" s="12"/>
-      <c r="M22" s="22"/>
-      <c r="N22" s="12"/>
-      <c r="O22" s="11"/>
-      <c r="P22" s="12"/>
+      <c r="L22" s="13"/>
+      <c r="M22" s="12"/>
+      <c r="N22" s="13"/>
+      <c r="O22" s="14"/>
+      <c r="P22" s="13"/>
       <c r="Q22" s="8" t="s">
         <v>77</v>
       </c>
@@ -1607,14 +1613,14 @@
       <c r="D23" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="E23" s="11"/>
+      <c r="E23" s="14"/>
       <c r="F23" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="G23" s="13" t="s">
+      <c r="G23" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="H23" s="14" t="s">
+      <c r="H23" s="16" t="s">
         <v>49</v>
       </c>
       <c r="I23" s="1"/>
@@ -1631,14 +1637,14 @@
       <c r="N23" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="O23" s="11"/>
+      <c r="O23" s="14"/>
       <c r="P23" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="Q23" s="13" t="s">
+      <c r="Q23" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="R23" s="14" t="s">
+      <c r="R23" s="16" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1646,13 +1652,13 @@
       <c r="A24" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B24" s="14" t="s">
+      <c r="B24" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="C24" s="14" t="s">
+      <c r="C24" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="D24" s="14" t="s">
+      <c r="D24" s="16" t="s">
         <v>49</v>
       </c>
       <c r="E24" s="8" t="s">
@@ -1661,20 +1667,20 @@
       <c r="F24" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="G24" s="13"/>
-      <c r="H24" s="14"/>
+      <c r="G24" s="15"/>
+      <c r="H24" s="16"/>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
       <c r="K24" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="L24" s="14" t="s">
+      <c r="L24" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="M24" s="14" t="s">
+      <c r="M24" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="N24" s="14" t="s">
+      <c r="N24" s="16" t="s">
         <v>49</v>
       </c>
       <c r="O24" s="8" t="s">
@@ -1683,44 +1689,44 @@
       <c r="P24" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="Q24" s="13"/>
-      <c r="R24" s="14"/>
+      <c r="Q24" s="15"/>
+      <c r="R24" s="16"/>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B25" s="14"/>
-      <c r="C25" s="14"/>
-      <c r="D25" s="14"/>
+      <c r="B25" s="16"/>
+      <c r="C25" s="16"/>
+      <c r="D25" s="16"/>
       <c r="E25" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="F25" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="G25" s="15" t="s">
+      <c r="F25" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="G25" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="H25" s="14"/>
+      <c r="H25" s="16"/>
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
       <c r="K25" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="L25" s="14"/>
-      <c r="M25" s="14"/>
-      <c r="N25" s="14"/>
+      <c r="L25" s="16"/>
+      <c r="M25" s="16"/>
+      <c r="N25" s="16"/>
       <c r="O25" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="P25" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q25" s="15" t="s">
+      <c r="P25" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q25" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="R25" s="14"/>
+      <c r="R25" s="16"/>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
@@ -1738,8 +1744,8 @@
       <c r="E26" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="F26" s="15"/>
-      <c r="G26" s="15"/>
+      <c r="F26" s="17"/>
+      <c r="G26" s="17"/>
       <c r="H26" s="10" t="s">
         <v>32</v>
       </c>
@@ -1760,8 +1766,8 @@
       <c r="O26" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="P26" s="15"/>
-      <c r="Q26" s="15"/>
+      <c r="P26" s="17"/>
+      <c r="Q26" s="17"/>
       <c r="R26" s="10" t="s">
         <v>32</v>
       </c>
@@ -2034,19 +2040,19 @@
       <c r="A38" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B38" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="C38" s="11" t="s">
+      <c r="B38" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C38" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="D38" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="E38" s="11" t="s">
+      <c r="D38" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E38" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="F38" s="19" t="s">
+      <c r="F38" s="11" t="s">
         <v>33</v>
       </c>
       <c r="G38" s="23"/>
@@ -2054,19 +2060,19 @@
       <c r="K38" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="L38" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="M38" s="11" t="s">
+      <c r="L38" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="M38" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="N38" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="O38" s="11" t="s">
+      <c r="N38" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="O38" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="P38" s="19" t="s">
+      <c r="P38" s="11" t="s">
         <v>33</v>
       </c>
       <c r="Q38" s="23"/>
@@ -2076,21 +2082,21 @@
       <c r="A39" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B39" s="22"/>
-      <c r="C39" s="11"/>
-      <c r="D39" s="22"/>
-      <c r="E39" s="11"/>
-      <c r="F39" s="22"/>
+      <c r="B39" s="12"/>
+      <c r="C39" s="14"/>
+      <c r="D39" s="12"/>
+      <c r="E39" s="14"/>
+      <c r="F39" s="12"/>
       <c r="G39" s="5"/>
       <c r="H39" s="5"/>
       <c r="K39" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="L39" s="22"/>
-      <c r="M39" s="11"/>
-      <c r="N39" s="22"/>
-      <c r="O39" s="11"/>
-      <c r="P39" s="22"/>
+      <c r="L39" s="12"/>
+      <c r="M39" s="14"/>
+      <c r="N39" s="12"/>
+      <c r="O39" s="14"/>
+      <c r="P39" s="12"/>
       <c r="Q39" s="5"/>
       <c r="R39" s="5"/>
     </row>
@@ -2098,49 +2104,49 @@
       <c r="A40" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B40" s="11" t="s">
+      <c r="B40" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="C40" s="11" t="s">
+      <c r="C40" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="D40" s="11" t="s">
+      <c r="D40" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="E40" s="11" t="s">
+      <c r="E40" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="F40" s="11" t="s">
+      <c r="F40" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="G40" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="H40" s="19" t="s">
+      <c r="G40" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="H40" s="11" t="s">
         <v>33</v>
       </c>
       <c r="K40" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L40" s="11" t="s">
+      <c r="L40" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="M40" s="11" t="s">
+      <c r="M40" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="N40" s="11" t="s">
+      <c r="N40" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="O40" s="11" t="s">
+      <c r="O40" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="P40" s="11" t="s">
+      <c r="P40" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="Q40" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="R40" s="19" t="s">
+      <c r="Q40" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="R40" s="11" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2148,23 +2154,23 @@
       <c r="A41" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B41" s="11"/>
-      <c r="C41" s="11"/>
-      <c r="D41" s="11"/>
-      <c r="E41" s="11"/>
-      <c r="F41" s="11"/>
-      <c r="G41" s="19"/>
-      <c r="H41" s="19"/>
+      <c r="B41" s="14"/>
+      <c r="C41" s="14"/>
+      <c r="D41" s="14"/>
+      <c r="E41" s="14"/>
+      <c r="F41" s="14"/>
+      <c r="G41" s="11"/>
+      <c r="H41" s="11"/>
       <c r="K41" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="L41" s="11"/>
-      <c r="M41" s="11"/>
-      <c r="N41" s="11"/>
-      <c r="O41" s="11"/>
-      <c r="P41" s="11"/>
-      <c r="Q41" s="19"/>
-      <c r="R41" s="19"/>
+      <c r="L41" s="14"/>
+      <c r="M41" s="14"/>
+      <c r="N41" s="14"/>
+      <c r="O41" s="14"/>
+      <c r="P41" s="14"/>
+      <c r="Q41" s="11"/>
+      <c r="R41" s="11"/>
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
@@ -2173,40 +2179,40 @@
       <c r="B42" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C42" s="11" t="s">
+      <c r="C42" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="D42" s="11" t="s">
+      <c r="D42" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="E42" s="11" t="s">
+      <c r="E42" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="F42" s="11" t="s">
+      <c r="F42" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="G42" s="19"/>
-      <c r="H42" s="19"/>
+      <c r="G42" s="11"/>
+      <c r="H42" s="11"/>
       <c r="K42" s="3" t="s">
         <v>22</v>
       </c>
       <c r="L42" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="M42" s="11" t="s">
+      <c r="M42" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="N42" s="11" t="s">
+      <c r="N42" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="O42" s="11" t="s">
+      <c r="O42" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="P42" s="11" t="s">
+      <c r="P42" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="Q42" s="19"/>
-      <c r="R42" s="19"/>
+      <c r="Q42" s="11"/>
+      <c r="R42" s="11"/>
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
@@ -2215,24 +2221,24 @@
       <c r="B43" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C43" s="11"/>
-      <c r="D43" s="11"/>
-      <c r="E43" s="11"/>
-      <c r="F43" s="11"/>
-      <c r="G43" s="19"/>
-      <c r="H43" s="19"/>
+      <c r="C43" s="14"/>
+      <c r="D43" s="14"/>
+      <c r="E43" s="14"/>
+      <c r="F43" s="14"/>
+      <c r="G43" s="11"/>
+      <c r="H43" s="11"/>
       <c r="K43" s="3" t="s">
         <v>21</v>
       </c>
       <c r="L43" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="M43" s="11"/>
-      <c r="N43" s="11"/>
-      <c r="O43" s="11"/>
-      <c r="P43" s="11"/>
-      <c r="Q43" s="19"/>
-      <c r="R43" s="19"/>
+      <c r="M43" s="14"/>
+      <c r="N43" s="14"/>
+      <c r="O43" s="14"/>
+      <c r="P43" s="14"/>
+      <c r="Q43" s="11"/>
+      <c r="R43" s="11"/>
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
@@ -2288,49 +2294,49 @@
       <c r="A45" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B45" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="C45" s="19" t="s">
+      <c r="B45" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C45" s="11" t="s">
         <v>33</v>
       </c>
       <c r="D45" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="E45" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="F45" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="G45" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="H45" s="16" t="s">
+      <c r="E45" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F45" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="G45" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="H45" s="18" t="s">
         <v>33</v>
       </c>
       <c r="K45" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="L45" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="M45" s="19" t="s">
+      <c r="L45" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="M45" s="11" t="s">
         <v>33</v>
       </c>
       <c r="N45" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="O45" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="P45" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q45" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="R45" s="16" t="s">
+      <c r="O45" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="P45" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q45" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="R45" s="18" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2338,111 +2344,111 @@
       <c r="A46" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B46" s="19"/>
-      <c r="C46" s="19"/>
-      <c r="D46" s="11" t="s">
+      <c r="B46" s="11"/>
+      <c r="C46" s="11"/>
+      <c r="D46" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="E46" s="19"/>
-      <c r="F46" s="19"/>
-      <c r="G46" s="17"/>
-      <c r="H46" s="17"/>
+      <c r="E46" s="11"/>
+      <c r="F46" s="11"/>
+      <c r="G46" s="19"/>
+      <c r="H46" s="19"/>
       <c r="K46" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="L46" s="19"/>
-      <c r="M46" s="19"/>
-      <c r="N46" s="11" t="s">
+      <c r="L46" s="11"/>
+      <c r="M46" s="11"/>
+      <c r="N46" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="O46" s="19"/>
-      <c r="P46" s="19"/>
-      <c r="Q46" s="17"/>
-      <c r="R46" s="17"/>
+      <c r="O46" s="11"/>
+      <c r="P46" s="11"/>
+      <c r="Q46" s="19"/>
+      <c r="R46" s="19"/>
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B47" s="11" t="s">
+      <c r="B47" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="C47" s="11" t="s">
+      <c r="C47" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="D47" s="11"/>
-      <c r="E47" s="19"/>
-      <c r="F47" s="11" t="s">
+      <c r="D47" s="14"/>
+      <c r="E47" s="11"/>
+      <c r="F47" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="G47" s="17"/>
-      <c r="H47" s="17"/>
+      <c r="G47" s="19"/>
+      <c r="H47" s="19"/>
       <c r="K47" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="L47" s="11" t="s">
+      <c r="L47" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="M47" s="11" t="s">
+      <c r="M47" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="N47" s="11"/>
-      <c r="O47" s="19"/>
-      <c r="P47" s="11" t="s">
+      <c r="N47" s="14"/>
+      <c r="O47" s="11"/>
+      <c r="P47" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="Q47" s="17"/>
-      <c r="R47" s="17"/>
+      <c r="Q47" s="19"/>
+      <c r="R47" s="19"/>
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B48" s="11"/>
-      <c r="C48" s="11"/>
-      <c r="D48" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="E48" s="19"/>
-      <c r="F48" s="11"/>
-      <c r="G48" s="17"/>
-      <c r="H48" s="18"/>
+      <c r="B48" s="14"/>
+      <c r="C48" s="14"/>
+      <c r="D48" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E48" s="11"/>
+      <c r="F48" s="14"/>
+      <c r="G48" s="19"/>
+      <c r="H48" s="20"/>
       <c r="K48" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="L48" s="11"/>
-      <c r="M48" s="11"/>
-      <c r="N48" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="O48" s="19"/>
-      <c r="P48" s="11"/>
-      <c r="Q48" s="17"/>
-      <c r="R48" s="18"/>
+      <c r="L48" s="14"/>
+      <c r="M48" s="14"/>
+      <c r="N48" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="O48" s="11"/>
+      <c r="P48" s="14"/>
+      <c r="Q48" s="19"/>
+      <c r="R48" s="20"/>
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B49" s="11"/>
-      <c r="C49" s="11"/>
-      <c r="D49" s="19"/>
-      <c r="E49" s="19"/>
-      <c r="F49" s="11"/>
-      <c r="G49" s="18"/>
-      <c r="H49" s="20" t="s">
+      <c r="B49" s="14"/>
+      <c r="C49" s="14"/>
+      <c r="D49" s="11"/>
+      <c r="E49" s="11"/>
+      <c r="F49" s="14"/>
+      <c r="G49" s="20"/>
+      <c r="H49" s="21" t="s">
         <v>53</v>
       </c>
       <c r="K49" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="L49" s="11"/>
-      <c r="M49" s="11"/>
-      <c r="N49" s="19"/>
-      <c r="O49" s="19"/>
-      <c r="P49" s="11"/>
-      <c r="Q49" s="18"/>
-      <c r="R49" s="20" t="s">
+      <c r="L49" s="14"/>
+      <c r="M49" s="14"/>
+      <c r="N49" s="11"/>
+      <c r="O49" s="11"/>
+      <c r="P49" s="14"/>
+      <c r="Q49" s="20"/>
+      <c r="R49" s="21" t="s">
         <v>53</v>
       </c>
     </row>
@@ -2450,57 +2456,57 @@
       <c r="A50" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B50" s="12" t="s">
+      <c r="B50" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="C50" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="D50" s="12" t="s">
+      <c r="C50" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D50" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="E50" s="11" t="s">
+      <c r="E50" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="F50" s="12" t="s">
+      <c r="F50" s="13" t="s">
         <v>43</v>
       </c>
       <c r="G50" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="H50" s="21"/>
+      <c r="H50" s="22"/>
       <c r="K50" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="L50" s="12" t="s">
+      <c r="L50" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="M50" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="N50" s="12" t="s">
+      <c r="M50" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="N50" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="O50" s="11" t="s">
+      <c r="O50" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="P50" s="12" t="s">
+      <c r="P50" s="13" t="s">
         <v>43</v>
       </c>
       <c r="Q50" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="R50" s="21"/>
+      <c r="R50" s="22"/>
     </row>
     <row r="51" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B51" s="12"/>
-      <c r="C51" s="22"/>
-      <c r="D51" s="12"/>
-      <c r="E51" s="11"/>
-      <c r="F51" s="12"/>
+      <c r="B51" s="13"/>
+      <c r="C51" s="12"/>
+      <c r="D51" s="13"/>
+      <c r="E51" s="14"/>
+      <c r="F51" s="13"/>
       <c r="G51" s="8" t="s">
         <v>36</v>
       </c>
@@ -2510,11 +2516,11 @@
       <c r="K51" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="L51" s="12"/>
-      <c r="M51" s="22"/>
-      <c r="N51" s="12"/>
-      <c r="O51" s="11"/>
-      <c r="P51" s="12"/>
+      <c r="L51" s="13"/>
+      <c r="M51" s="12"/>
+      <c r="N51" s="13"/>
+      <c r="O51" s="14"/>
+      <c r="P51" s="13"/>
       <c r="Q51" s="8" t="s">
         <v>81</v>
       </c>
@@ -2535,11 +2541,11 @@
       <c r="D52" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="E52" s="11"/>
+      <c r="E52" s="14"/>
       <c r="F52" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="G52" s="13" t="s">
+      <c r="G52" s="15" t="s">
         <v>51</v>
       </c>
       <c r="H52" s="24" t="s">
@@ -2557,14 +2563,14 @@
       <c r="N52" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="O52" s="11"/>
+      <c r="O52" s="14"/>
       <c r="P52" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="Q52" s="13" t="s">
+      <c r="Q52" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="R52" s="14" t="s">
+      <c r="R52" s="16" t="s">
         <v>49</v>
       </c>
     </row>
@@ -2572,13 +2578,13 @@
       <c r="A53" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B53" s="14" t="s">
+      <c r="B53" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="C53" s="14" t="s">
+      <c r="C53" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="D53" s="14" t="s">
+      <c r="D53" s="16" t="s">
         <v>49</v>
       </c>
       <c r="E53" s="8" t="s">
@@ -2587,18 +2593,18 @@
       <c r="F53" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="G53" s="13"/>
-      <c r="H53" s="26"/>
+      <c r="G53" s="15"/>
+      <c r="H53" s="25"/>
       <c r="K53" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="L53" s="14" t="s">
+      <c r="L53" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="M53" s="14" t="s">
+      <c r="M53" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="N53" s="14" t="s">
+      <c r="N53" s="16" t="s">
         <v>49</v>
       </c>
       <c r="O53" s="8" t="s">
@@ -2607,42 +2613,42 @@
       <c r="P53" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="Q53" s="13"/>
-      <c r="R53" s="14"/>
+      <c r="Q53" s="15"/>
+      <c r="R53" s="16"/>
     </row>
     <row r="54" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B54" s="14"/>
-      <c r="C54" s="14"/>
-      <c r="D54" s="14"/>
+      <c r="B54" s="16"/>
+      <c r="C54" s="16"/>
+      <c r="D54" s="16"/>
       <c r="E54" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="F54" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="G54" s="15" t="s">
+      <c r="F54" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="G54" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="H54" s="25"/>
+      <c r="H54" s="26"/>
       <c r="K54" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="L54" s="14"/>
-      <c r="M54" s="14"/>
-      <c r="N54" s="14"/>
+      <c r="L54" s="16"/>
+      <c r="M54" s="16"/>
+      <c r="N54" s="16"/>
       <c r="O54" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="P54" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q54" s="15" t="s">
+      <c r="P54" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q54" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="R54" s="14"/>
+      <c r="R54" s="16"/>
     </row>
     <row r="55" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
@@ -2660,8 +2666,8 @@
       <c r="E55" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="F55" s="15"/>
-      <c r="G55" s="15"/>
+      <c r="F55" s="17"/>
+      <c r="G55" s="17"/>
       <c r="H55" s="10" t="s">
         <v>32</v>
       </c>
@@ -2680,14 +2686,23 @@
       <c r="O55" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="P55" s="15"/>
-      <c r="Q55" s="15"/>
+      <c r="P55" s="17"/>
+      <c r="Q55" s="17"/>
       <c r="R55" s="10" t="s">
         <v>32</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="188">
+    <mergeCell ref="H45:H48"/>
+    <mergeCell ref="H49:H50"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="C11:C12"/>
     <mergeCell ref="H52:H54"/>
     <mergeCell ref="C3:C7"/>
     <mergeCell ref="D3:D7"/>
@@ -2697,33 +2712,24 @@
     <mergeCell ref="D13:D14"/>
     <mergeCell ref="E13:E14"/>
     <mergeCell ref="F13:F14"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="F21:F22"/>
-    <mergeCell ref="C18:C20"/>
-    <mergeCell ref="F18:F20"/>
-    <mergeCell ref="E21:E23"/>
-    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="F25:F26"/>
+    <mergeCell ref="H32:H38"/>
+    <mergeCell ref="G32:G38"/>
+    <mergeCell ref="H40:H43"/>
+    <mergeCell ref="C42:C43"/>
+    <mergeCell ref="D42:D43"/>
     <mergeCell ref="B3:B7"/>
     <mergeCell ref="B9:B10"/>
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="B18:B20"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="F25:F26"/>
     <mergeCell ref="C21:C22"/>
     <mergeCell ref="D19:D20"/>
     <mergeCell ref="E16:E20"/>
     <mergeCell ref="B16:B17"/>
     <mergeCell ref="C16:C17"/>
     <mergeCell ref="D9:D10"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="C11:C12"/>
     <mergeCell ref="B24:B25"/>
     <mergeCell ref="G23:G24"/>
     <mergeCell ref="G25:G26"/>
@@ -2738,6 +2744,16 @@
     <mergeCell ref="H11:H14"/>
     <mergeCell ref="G3:G9"/>
     <mergeCell ref="H3:H9"/>
+    <mergeCell ref="H16:H19"/>
+    <mergeCell ref="H20:H21"/>
+    <mergeCell ref="G16:G20"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="C18:C20"/>
+    <mergeCell ref="F18:F20"/>
+    <mergeCell ref="E21:E23"/>
+    <mergeCell ref="D17:D18"/>
     <mergeCell ref="M3:M7"/>
     <mergeCell ref="N3:N7"/>
     <mergeCell ref="O3:O7"/>
@@ -2759,12 +2775,15 @@
     <mergeCell ref="N13:N14"/>
     <mergeCell ref="O13:O14"/>
     <mergeCell ref="P13:P14"/>
-    <mergeCell ref="H16:H19"/>
-    <mergeCell ref="H20:H21"/>
-    <mergeCell ref="G16:G20"/>
     <mergeCell ref="Q16:Q20"/>
     <mergeCell ref="R16:R19"/>
     <mergeCell ref="R20:R21"/>
+    <mergeCell ref="M16:M17"/>
+    <mergeCell ref="O16:O20"/>
+    <mergeCell ref="P16:P17"/>
+    <mergeCell ref="N17:N18"/>
+    <mergeCell ref="M18:M20"/>
+    <mergeCell ref="P18:P20"/>
     <mergeCell ref="R23:R25"/>
     <mergeCell ref="L24:L25"/>
     <mergeCell ref="M24:M25"/>
@@ -2777,13 +2796,6 @@
     <mergeCell ref="O21:O23"/>
     <mergeCell ref="P21:P22"/>
     <mergeCell ref="Q23:Q24"/>
-    <mergeCell ref="M16:M17"/>
-    <mergeCell ref="O16:O20"/>
-    <mergeCell ref="P16:P17"/>
-    <mergeCell ref="N17:N18"/>
-    <mergeCell ref="M18:M20"/>
-    <mergeCell ref="P18:P20"/>
-    <mergeCell ref="H32:H38"/>
     <mergeCell ref="B38:B39"/>
     <mergeCell ref="C38:C39"/>
     <mergeCell ref="D38:D39"/>
@@ -2794,12 +2806,6 @@
     <mergeCell ref="D32:D36"/>
     <mergeCell ref="E32:E36"/>
     <mergeCell ref="F32:F36"/>
-    <mergeCell ref="G32:G38"/>
-    <mergeCell ref="H40:H43"/>
-    <mergeCell ref="C42:C43"/>
-    <mergeCell ref="D42:D43"/>
-    <mergeCell ref="E42:E43"/>
-    <mergeCell ref="F42:F43"/>
     <mergeCell ref="B45:B46"/>
     <mergeCell ref="C45:C46"/>
     <mergeCell ref="E45:E49"/>
@@ -2811,13 +2817,13 @@
     <mergeCell ref="E40:E41"/>
     <mergeCell ref="F40:F41"/>
     <mergeCell ref="G40:G43"/>
-    <mergeCell ref="H45:H48"/>
     <mergeCell ref="D46:D47"/>
     <mergeCell ref="B47:B49"/>
     <mergeCell ref="C47:C49"/>
     <mergeCell ref="F47:F49"/>
     <mergeCell ref="D48:D49"/>
-    <mergeCell ref="H49:H50"/>
+    <mergeCell ref="E42:E43"/>
+    <mergeCell ref="F42:F43"/>
     <mergeCell ref="B50:B51"/>
     <mergeCell ref="C50:C51"/>
     <mergeCell ref="D50:D51"/>

</xml_diff>

<commit_message>
Cambio actividades de fin de semana
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MATEO\Desktop\Platzi\Curso Git - GutHub\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MATEO\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{202A588B-B73A-40D4-BF99-684A8BFD0A6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D79D9D44-1D2A-4613-8931-82F30E1807D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{A899F46E-BA08-4AC6-A7C3-F03724044CD5}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="88">
   <si>
     <t>Hora</t>
   </si>
@@ -290,10 +290,16 @@
     <t>Cena - Guardar Ropa</t>
   </si>
   <si>
-    <t>Proyecto de redes 1</t>
-  </si>
-  <si>
-    <t>Practica 1 Analogica 2</t>
+    <t xml:space="preserve">Clases de tecnicas </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tarea tecnicas </t>
+  </si>
+  <si>
+    <t>Estudio Digital 2</t>
+  </si>
+  <si>
+    <t>Compras - Cena</t>
   </si>
 </sst>
 </file>
@@ -439,7 +445,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -469,25 +475,37 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -505,16 +523,13 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -833,8 +848,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9132D586-DE4C-4B7E-830E-683E06A9C036}">
   <dimension ref="A2:R55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13:C14"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="117" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12:G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -881,7 +896,9 @@
       <c r="H2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="1"/>
+      <c r="I2" s="2" t="s">
+        <v>0</v>
+      </c>
       <c r="J2" s="1"/>
       <c r="K2" s="2" t="s">
         <v>0</v>
@@ -912,51 +929,53 @@
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="C3" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="D3" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="E3" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="F3" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="G3" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="H3" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="I3" s="1"/>
+      <c r="B3" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="G3" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="H3" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="J3" s="1"/>
       <c r="K3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="L3" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="M3" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="N3" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="O3" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="P3" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q3" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="R3" s="23" t="s">
+      <c r="L3" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="M3" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="N3" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="O3" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="P3" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q3" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="R3" s="14" t="s">
         <v>32</v>
       </c>
     </row>
@@ -964,97 +983,105 @@
       <c r="A4" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="23"/>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="23"/>
-      <c r="F4" s="23"/>
-      <c r="G4" s="23"/>
-      <c r="H4" s="23"/>
-      <c r="I4" s="1"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="28"/>
+      <c r="H4" s="28"/>
+      <c r="I4" s="3" t="s">
+        <v>31</v>
+      </c>
       <c r="J4" s="1"/>
       <c r="K4" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="L4" s="23"/>
-      <c r="M4" s="23"/>
-      <c r="N4" s="23"/>
-      <c r="O4" s="23"/>
-      <c r="P4" s="23"/>
-      <c r="Q4" s="23"/>
-      <c r="R4" s="23"/>
+      <c r="L4" s="14"/>
+      <c r="M4" s="14"/>
+      <c r="N4" s="14"/>
+      <c r="O4" s="14"/>
+      <c r="P4" s="14"/>
+      <c r="Q4" s="14"/>
+      <c r="R4" s="14"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="23"/>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="23"/>
-      <c r="G5" s="23"/>
-      <c r="H5" s="23"/>
-      <c r="I5" s="1"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="28"/>
+      <c r="H5" s="28"/>
+      <c r="I5" s="3" t="s">
+        <v>30</v>
+      </c>
       <c r="J5" s="1"/>
       <c r="K5" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="L5" s="23"/>
-      <c r="M5" s="23"/>
-      <c r="N5" s="23"/>
-      <c r="O5" s="23"/>
-      <c r="P5" s="23"/>
-      <c r="Q5" s="23"/>
-      <c r="R5" s="23"/>
+      <c r="L5" s="14"/>
+      <c r="M5" s="14"/>
+      <c r="N5" s="14"/>
+      <c r="O5" s="14"/>
+      <c r="P5" s="14"/>
+      <c r="Q5" s="14"/>
+      <c r="R5" s="14"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B6" s="23"/>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="23"/>
-      <c r="G6" s="23"/>
-      <c r="H6" s="23"/>
-      <c r="I6" s="1"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="28"/>
+      <c r="H6" s="28"/>
+      <c r="I6" s="3" t="s">
+        <v>29</v>
+      </c>
       <c r="J6" s="1"/>
       <c r="K6" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="L6" s="23"/>
-      <c r="M6" s="23"/>
-      <c r="N6" s="23"/>
-      <c r="O6" s="23"/>
-      <c r="P6" s="23"/>
-      <c r="Q6" s="23"/>
-      <c r="R6" s="23"/>
+      <c r="L6" s="14"/>
+      <c r="M6" s="14"/>
+      <c r="N6" s="14"/>
+      <c r="O6" s="14"/>
+      <c r="P6" s="14"/>
+      <c r="Q6" s="14"/>
+      <c r="R6" s="14"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="23"/>
-      <c r="C7" s="23"/>
-      <c r="D7" s="23"/>
-      <c r="E7" s="23"/>
-      <c r="F7" s="23"/>
-      <c r="G7" s="23"/>
-      <c r="H7" s="23"/>
-      <c r="I7" s="1"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="28"/>
+      <c r="H7" s="28"/>
+      <c r="I7" s="3" t="s">
+        <v>28</v>
+      </c>
       <c r="J7" s="1"/>
       <c r="K7" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="L7" s="23"/>
-      <c r="M7" s="23"/>
-      <c r="N7" s="23"/>
-      <c r="O7" s="23"/>
-      <c r="P7" s="23"/>
-      <c r="Q7" s="23"/>
-      <c r="R7" s="23"/>
+      <c r="L7" s="14"/>
+      <c r="M7" s="14"/>
+      <c r="N7" s="14"/>
+      <c r="O7" s="14"/>
+      <c r="P7" s="14"/>
+      <c r="Q7" s="14"/>
+      <c r="R7" s="14"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
@@ -1065,9 +1092,11 @@
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
-      <c r="G8" s="23"/>
-      <c r="H8" s="23"/>
-      <c r="I8" s="1"/>
+      <c r="G8" s="29"/>
+      <c r="H8" s="29"/>
+      <c r="I8" s="3" t="s">
+        <v>27</v>
+      </c>
       <c r="J8" s="1"/>
       <c r="K8" s="3" t="s">
         <v>27</v>
@@ -1077,74 +1106,82 @@
       <c r="N8" s="5"/>
       <c r="O8" s="5"/>
       <c r="P8" s="5"/>
-      <c r="Q8" s="23"/>
-      <c r="R8" s="23"/>
+      <c r="Q8" s="14"/>
+      <c r="R8" s="14"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="C9" s="14" t="s">
+      <c r="B9" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="D9" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="E9" s="14" t="s">
+      <c r="D9" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="F9" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="G9" s="23"/>
-      <c r="H9" s="23"/>
-      <c r="I9" s="1"/>
+      <c r="F9" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="3" t="s">
+        <v>26</v>
+      </c>
       <c r="J9" s="1"/>
       <c r="K9" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="L9" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="M9" s="14" t="s">
+      <c r="L9" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="M9" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="N9" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="O9" s="14" t="s">
+      <c r="N9" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="O9" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="P9" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q9" s="23"/>
-      <c r="R9" s="23"/>
+      <c r="P9" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q9" s="14"/>
+      <c r="R9" s="14"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="12"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="1"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="H10" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="J10" s="1"/>
       <c r="K10" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="L10" s="12"/>
-      <c r="M10" s="14"/>
-      <c r="N10" s="12"/>
-      <c r="O10" s="14"/>
-      <c r="P10" s="12"/>
+      <c r="L10" s="18"/>
+      <c r="M10" s="15"/>
+      <c r="N10" s="18"/>
+      <c r="O10" s="15"/>
+      <c r="P10" s="18"/>
       <c r="Q10" s="5"/>
       <c r="R10" s="5"/>
     </row>
@@ -1152,51 +1189,49 @@
       <c r="A11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="C11" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="D11" s="14" t="s">
+      <c r="D11" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="E11" s="14" t="s">
+      <c r="E11" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="F11" s="14" t="s">
+      <c r="F11" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="G11" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="H11" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="I11" s="1"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="23"/>
+      <c r="I11" s="3" t="s">
+        <v>24</v>
+      </c>
       <c r="J11" s="1"/>
       <c r="K11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L11" s="14" t="s">
+      <c r="L11" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="M11" s="14" t="s">
+      <c r="M11" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="N11" s="14" t="s">
+      <c r="N11" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="O11" s="14" t="s">
+      <c r="O11" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="P11" s="14" t="s">
+      <c r="P11" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="Q11" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="R11" s="11" t="s">
+      <c r="Q11" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="R11" s="17" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1204,48 +1239,54 @@
       <c r="A12" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="14"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="1"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="H12" s="23"/>
+      <c r="I12" s="3" t="s">
+        <v>23</v>
+      </c>
       <c r="J12" s="1"/>
       <c r="K12" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="L12" s="14"/>
-      <c r="M12" s="14"/>
-      <c r="N12" s="14"/>
-      <c r="O12" s="14"/>
-      <c r="P12" s="14"/>
-      <c r="Q12" s="11"/>
-      <c r="R12" s="11"/>
+      <c r="L12" s="15"/>
+      <c r="M12" s="15"/>
+      <c r="N12" s="15"/>
+      <c r="O12" s="15"/>
+      <c r="P12" s="15"/>
+      <c r="Q12" s="17"/>
+      <c r="R12" s="17"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="C13" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="D13" s="14" t="s">
+      <c r="D13" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="E13" s="14" t="s">
+      <c r="E13" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="F13" s="14" t="s">
+      <c r="F13" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="G13" s="11"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="1"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="23"/>
+      <c r="I13" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="J13" s="1"/>
       <c r="K13" s="3" t="s">
         <v>22</v>
@@ -1253,20 +1294,20 @@
       <c r="L13" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="M13" s="14" t="s">
+      <c r="M13" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="N13" s="14" t="s">
+      <c r="N13" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="O13" s="14" t="s">
+      <c r="O13" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="P13" s="14" t="s">
+      <c r="P13" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="Q13" s="11"/>
-      <c r="R13" s="11"/>
+      <c r="Q13" s="17"/>
+      <c r="R13" s="17"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
@@ -1275,13 +1316,17 @@
       <c r="B14" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="11"/>
-      <c r="I14" s="1"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="H14" s="24"/>
+      <c r="I14" s="3" t="s">
+        <v>21</v>
+      </c>
       <c r="J14" s="1"/>
       <c r="K14" s="3" t="s">
         <v>21</v>
@@ -1289,12 +1334,12 @@
       <c r="L14" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="M14" s="14"/>
-      <c r="N14" s="14"/>
-      <c r="O14" s="14"/>
-      <c r="P14" s="14"/>
-      <c r="Q14" s="11"/>
-      <c r="R14" s="11"/>
+      <c r="M14" s="15"/>
+      <c r="N14" s="15"/>
+      <c r="O14" s="15"/>
+      <c r="P14" s="15"/>
+      <c r="Q14" s="17"/>
+      <c r="R14" s="17"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
@@ -1321,7 +1366,9 @@
       <c r="H15" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="I15" s="1"/>
+      <c r="I15" s="3" t="s">
+        <v>20</v>
+      </c>
       <c r="J15" s="1"/>
       <c r="K15" s="3" t="s">
         <v>20</v>
@@ -1352,51 +1399,53 @@
       <c r="A16" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="C16" s="11" t="s">
+      <c r="B16" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="17" t="s">
         <v>33</v>
       </c>
       <c r="D16" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="E16" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="F16" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="G16" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="H16" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="I16" s="1"/>
+      <c r="E16" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="F16" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="G16" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="H16" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="J16" s="1"/>
       <c r="K16" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="L16" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="M16" s="11" t="s">
+      <c r="L16" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="M16" s="17" t="s">
         <v>33</v>
       </c>
       <c r="N16" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="O16" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="P16" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q16" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="R16" s="18" t="s">
+      <c r="O16" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="P16" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q16" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="R16" s="22" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1404,119 +1453,129 @@
       <c r="A17" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="11"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="14" t="s">
+      <c r="B17" s="17"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="19"/>
-      <c r="H17" s="19"/>
-      <c r="I17" s="1"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="23"/>
+      <c r="H17" s="23"/>
+      <c r="I17" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="J17" s="1"/>
       <c r="K17" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="L17" s="11"/>
-      <c r="M17" s="11"/>
-      <c r="N17" s="14" t="s">
+      <c r="L17" s="17"/>
+      <c r="M17" s="17"/>
+      <c r="N17" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="O17" s="11"/>
-      <c r="P17" s="11"/>
-      <c r="Q17" s="19"/>
-      <c r="R17" s="19"/>
+      <c r="O17" s="17"/>
+      <c r="P17" s="17"/>
+      <c r="Q17" s="23"/>
+      <c r="R17" s="23"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="14" t="s">
+      <c r="B18" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="C18" s="14" t="s">
+      <c r="C18" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="D18" s="14"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="14" t="s">
+      <c r="D18" s="15"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="G18" s="19"/>
-      <c r="H18" s="19"/>
-      <c r="I18" s="1"/>
+      <c r="G18" s="22" t="s">
+        <v>86</v>
+      </c>
+      <c r="H18" s="23"/>
+      <c r="I18" s="3" t="s">
+        <v>17</v>
+      </c>
       <c r="J18" s="1"/>
       <c r="K18" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="L18" s="14" t="s">
+      <c r="L18" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="M18" s="14" t="s">
+      <c r="M18" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="N18" s="14"/>
-      <c r="O18" s="11"/>
-      <c r="P18" s="14" t="s">
+      <c r="N18" s="15"/>
+      <c r="O18" s="17"/>
+      <c r="P18" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="Q18" s="19"/>
-      <c r="R18" s="19"/>
+      <c r="Q18" s="23"/>
+      <c r="R18" s="23"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="14"/>
-      <c r="C19" s="14"/>
-      <c r="D19" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="E19" s="11"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="19"/>
-      <c r="H19" s="20"/>
-      <c r="I19" s="1"/>
+      <c r="B19" s="15"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="E19" s="17"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="23"/>
+      <c r="H19" s="24"/>
+      <c r="I19" s="3" t="s">
+        <v>16</v>
+      </c>
       <c r="J19" s="1"/>
       <c r="K19" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="L19" s="14"/>
-      <c r="M19" s="14"/>
-      <c r="N19" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="O19" s="11"/>
-      <c r="P19" s="14"/>
-      <c r="Q19" s="19"/>
-      <c r="R19" s="20"/>
+      <c r="L19" s="15"/>
+      <c r="M19" s="15"/>
+      <c r="N19" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="O19" s="17"/>
+      <c r="P19" s="15"/>
+      <c r="Q19" s="23"/>
+      <c r="R19" s="24"/>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="14"/>
-      <c r="C20" s="14"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="20"/>
-      <c r="H20" s="21" t="s">
+      <c r="B20" s="15"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="23"/>
+      <c r="H20" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="I20" s="1"/>
+      <c r="I20" s="3" t="s">
+        <v>14</v>
+      </c>
       <c r="J20" s="1"/>
       <c r="K20" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="L20" s="14"/>
-      <c r="M20" s="14"/>
-      <c r="N20" s="11"/>
-      <c r="O20" s="11"/>
-      <c r="P20" s="14"/>
-      <c r="Q20" s="20"/>
-      <c r="R20" s="21" t="s">
+      <c r="L20" s="15"/>
+      <c r="M20" s="15"/>
+      <c r="N20" s="17"/>
+      <c r="O20" s="17"/>
+      <c r="P20" s="15"/>
+      <c r="Q20" s="24"/>
+      <c r="R20" s="25" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1524,75 +1583,77 @@
       <c r="A21" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B21" s="13" t="s">
+      <c r="B21" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="C21" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="D21" s="13" t="s">
+      <c r="C21" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="D21" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="E21" s="14" t="s">
+      <c r="E21" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="F21" s="13" t="s">
+      <c r="F21" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="G21" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="H21" s="22"/>
-      <c r="I21" s="1"/>
+      <c r="G21" s="24"/>
+      <c r="H21" s="26"/>
+      <c r="I21" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="J21" s="1"/>
       <c r="K21" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="L21" s="13" t="s">
+      <c r="L21" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="M21" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="N21" s="13" t="s">
+      <c r="M21" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="N21" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="O21" s="14" t="s">
+      <c r="O21" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="P21" s="13" t="s">
+      <c r="P21" s="16" t="s">
         <v>43</v>
       </c>
       <c r="Q21" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="R21" s="22"/>
+      <c r="R21" s="26"/>
     </row>
     <row r="22" spans="1:18" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B22" s="13"/>
-      <c r="C22" s="12"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="13"/>
+      <c r="B22" s="16"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="16"/>
       <c r="G22" s="8" t="s">
-        <v>36</v>
+        <v>87</v>
       </c>
       <c r="H22" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="I22" s="1"/>
+      <c r="I22" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="J22" s="1"/>
       <c r="K22" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="L22" s="13"/>
-      <c r="M22" s="12"/>
-      <c r="N22" s="13"/>
-      <c r="O22" s="14"/>
-      <c r="P22" s="13"/>
+      <c r="L22" s="16"/>
+      <c r="M22" s="18"/>
+      <c r="N22" s="16"/>
+      <c r="O22" s="15"/>
+      <c r="P22" s="16"/>
       <c r="Q22" s="8" t="s">
         <v>77</v>
       </c>
@@ -1613,17 +1674,19 @@
       <c r="D23" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="E23" s="14"/>
+      <c r="E23" s="15"/>
       <c r="F23" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="G23" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="H23" s="16" t="s">
+      <c r="G23" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="H23" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="I23" s="1"/>
+      <c r="I23" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="J23" s="1"/>
       <c r="K23" s="2" t="s">
         <v>10</v>
@@ -1637,14 +1700,14 @@
       <c r="N23" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="O23" s="14"/>
+      <c r="O23" s="15"/>
       <c r="P23" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="Q23" s="15" t="s">
+      <c r="Q23" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="R23" s="16" t="s">
+      <c r="R23" s="19" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1652,13 +1715,13 @@
       <c r="A24" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B24" s="16" t="s">
+      <c r="B24" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="C24" s="16" t="s">
+      <c r="C24" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="D24" s="16" t="s">
+      <c r="D24" s="19" t="s">
         <v>49</v>
       </c>
       <c r="E24" s="8" t="s">
@@ -1667,20 +1730,22 @@
       <c r="F24" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="G24" s="15"/>
-      <c r="H24" s="16"/>
-      <c r="I24" s="1"/>
+      <c r="G24" s="17"/>
+      <c r="H24" s="19"/>
+      <c r="I24" s="2" t="s">
+        <v>11</v>
+      </c>
       <c r="J24" s="1"/>
       <c r="K24" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="L24" s="16" t="s">
+      <c r="L24" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="M24" s="16" t="s">
+      <c r="M24" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="N24" s="16" t="s">
+      <c r="N24" s="19" t="s">
         <v>49</v>
       </c>
       <c r="O24" s="8" t="s">
@@ -1689,44 +1754,46 @@
       <c r="P24" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="Q24" s="15"/>
-      <c r="R24" s="16"/>
+      <c r="Q24" s="21"/>
+      <c r="R24" s="19"/>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B25" s="16"/>
-      <c r="C25" s="16"/>
-      <c r="D25" s="16"/>
+      <c r="B25" s="19"/>
+      <c r="C25" s="19"/>
+      <c r="D25" s="19"/>
       <c r="E25" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="F25" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="G25" s="17" t="s">
+      <c r="F25" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="G25" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="H25" s="16"/>
-      <c r="I25" s="1"/>
+      <c r="H25" s="19"/>
+      <c r="I25" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="J25" s="1"/>
       <c r="K25" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="L25" s="16"/>
-      <c r="M25" s="16"/>
-      <c r="N25" s="16"/>
+      <c r="L25" s="19"/>
+      <c r="M25" s="19"/>
+      <c r="N25" s="19"/>
       <c r="O25" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="P25" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q25" s="17" t="s">
+      <c r="P25" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q25" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="R25" s="16"/>
+      <c r="R25" s="19"/>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
@@ -1744,12 +1811,14 @@
       <c r="E26" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="F26" s="17"/>
-      <c r="G26" s="17"/>
+      <c r="F26" s="20"/>
+      <c r="G26" s="20"/>
       <c r="H26" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="I26" s="1"/>
+      <c r="I26" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="J26" s="1"/>
       <c r="K26" s="2" t="s">
         <v>13</v>
@@ -1766,8 +1835,8 @@
       <c r="O26" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="P26" s="17"/>
-      <c r="Q26" s="17"/>
+      <c r="P26" s="20"/>
+      <c r="Q26" s="20"/>
       <c r="R26" s="10" t="s">
         <v>32</v>
       </c>
@@ -1880,49 +1949,49 @@
       <c r="A32" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B32" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="C32" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="D32" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="E32" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="F32" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="G32" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="H32" s="23" t="s">
+      <c r="B32" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="C32" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="D32" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E32" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="F32" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="G32" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="H32" s="14" t="s">
         <v>32</v>
       </c>
       <c r="K32" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="L32" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="M32" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="N32" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="O32" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="P32" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q32" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="R32" s="23" t="s">
+      <c r="L32" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="M32" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="N32" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="O32" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="P32" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q32" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="R32" s="14" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1930,89 +1999,89 @@
       <c r="A33" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B33" s="23"/>
-      <c r="C33" s="23"/>
-      <c r="D33" s="23"/>
-      <c r="E33" s="23"/>
-      <c r="F33" s="23"/>
-      <c r="G33" s="23"/>
-      <c r="H33" s="23"/>
+      <c r="B33" s="14"/>
+      <c r="C33" s="14"/>
+      <c r="D33" s="14"/>
+      <c r="E33" s="14"/>
+      <c r="F33" s="14"/>
+      <c r="G33" s="14"/>
+      <c r="H33" s="14"/>
       <c r="K33" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="L33" s="23"/>
-      <c r="M33" s="23"/>
-      <c r="N33" s="23"/>
-      <c r="O33" s="23"/>
-      <c r="P33" s="23"/>
-      <c r="Q33" s="23"/>
-      <c r="R33" s="23"/>
+      <c r="L33" s="14"/>
+      <c r="M33" s="14"/>
+      <c r="N33" s="14"/>
+      <c r="O33" s="14"/>
+      <c r="P33" s="14"/>
+      <c r="Q33" s="14"/>
+      <c r="R33" s="14"/>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B34" s="23"/>
-      <c r="C34" s="23"/>
-      <c r="D34" s="23"/>
-      <c r="E34" s="23"/>
-      <c r="F34" s="23"/>
-      <c r="G34" s="23"/>
-      <c r="H34" s="23"/>
+      <c r="B34" s="14"/>
+      <c r="C34" s="14"/>
+      <c r="D34" s="14"/>
+      <c r="E34" s="14"/>
+      <c r="F34" s="14"/>
+      <c r="G34" s="14"/>
+      <c r="H34" s="14"/>
       <c r="K34" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="L34" s="23"/>
-      <c r="M34" s="23"/>
-      <c r="N34" s="23"/>
-      <c r="O34" s="23"/>
-      <c r="P34" s="23"/>
-      <c r="Q34" s="23"/>
-      <c r="R34" s="23"/>
+      <c r="L34" s="14"/>
+      <c r="M34" s="14"/>
+      <c r="N34" s="14"/>
+      <c r="O34" s="14"/>
+      <c r="P34" s="14"/>
+      <c r="Q34" s="14"/>
+      <c r="R34" s="14"/>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B35" s="23"/>
-      <c r="C35" s="23"/>
-      <c r="D35" s="23"/>
-      <c r="E35" s="23"/>
-      <c r="F35" s="23"/>
-      <c r="G35" s="23"/>
-      <c r="H35" s="23"/>
+      <c r="B35" s="14"/>
+      <c r="C35" s="14"/>
+      <c r="D35" s="14"/>
+      <c r="E35" s="14"/>
+      <c r="F35" s="14"/>
+      <c r="G35" s="14"/>
+      <c r="H35" s="14"/>
       <c r="K35" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="L35" s="23"/>
-      <c r="M35" s="23"/>
-      <c r="N35" s="23"/>
-      <c r="O35" s="23"/>
-      <c r="P35" s="23"/>
-      <c r="Q35" s="23"/>
-      <c r="R35" s="23"/>
+      <c r="L35" s="14"/>
+      <c r="M35" s="14"/>
+      <c r="N35" s="14"/>
+      <c r="O35" s="14"/>
+      <c r="P35" s="14"/>
+      <c r="Q35" s="14"/>
+      <c r="R35" s="14"/>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B36" s="23"/>
-      <c r="C36" s="23"/>
-      <c r="D36" s="23"/>
-      <c r="E36" s="23"/>
-      <c r="F36" s="23"/>
-      <c r="G36" s="23"/>
-      <c r="H36" s="23"/>
+      <c r="B36" s="14"/>
+      <c r="C36" s="14"/>
+      <c r="D36" s="14"/>
+      <c r="E36" s="14"/>
+      <c r="F36" s="14"/>
+      <c r="G36" s="14"/>
+      <c r="H36" s="14"/>
       <c r="K36" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="L36" s="23"/>
-      <c r="M36" s="23"/>
-      <c r="N36" s="23"/>
-      <c r="O36" s="23"/>
-      <c r="P36" s="23"/>
-      <c r="Q36" s="23"/>
-      <c r="R36" s="23"/>
+      <c r="L36" s="14"/>
+      <c r="M36" s="14"/>
+      <c r="N36" s="14"/>
+      <c r="O36" s="14"/>
+      <c r="P36" s="14"/>
+      <c r="Q36" s="14"/>
+      <c r="R36" s="14"/>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
@@ -2023,8 +2092,8 @@
       <c r="D37" s="5"/>
       <c r="E37" s="5"/>
       <c r="F37" s="5"/>
-      <c r="G37" s="23"/>
-      <c r="H37" s="23"/>
+      <c r="G37" s="14"/>
+      <c r="H37" s="14"/>
       <c r="K37" s="3" t="s">
         <v>27</v>
       </c>
@@ -2033,70 +2102,70 @@
       <c r="N37" s="5"/>
       <c r="O37" s="5"/>
       <c r="P37" s="5"/>
-      <c r="Q37" s="23"/>
-      <c r="R37" s="23"/>
+      <c r="Q37" s="14"/>
+      <c r="R37" s="14"/>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B38" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="C38" s="14" t="s">
+      <c r="B38" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="C38" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="D38" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="E38" s="14" t="s">
+      <c r="D38" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="E38" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="F38" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="G38" s="23"/>
-      <c r="H38" s="23"/>
+      <c r="F38" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="G38" s="14"/>
+      <c r="H38" s="14"/>
       <c r="K38" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="L38" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="M38" s="14" t="s">
+      <c r="L38" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="M38" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="N38" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="O38" s="14" t="s">
+      <c r="N38" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="O38" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="P38" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q38" s="23"/>
-      <c r="R38" s="23"/>
+      <c r="P38" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q38" s="14"/>
+      <c r="R38" s="14"/>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B39" s="12"/>
-      <c r="C39" s="14"/>
-      <c r="D39" s="12"/>
-      <c r="E39" s="14"/>
-      <c r="F39" s="12"/>
+      <c r="B39" s="18"/>
+      <c r="C39" s="15"/>
+      <c r="D39" s="18"/>
+      <c r="E39" s="15"/>
+      <c r="F39" s="18"/>
       <c r="G39" s="5"/>
       <c r="H39" s="5"/>
       <c r="K39" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="L39" s="12"/>
-      <c r="M39" s="14"/>
-      <c r="N39" s="12"/>
-      <c r="O39" s="14"/>
-      <c r="P39" s="12"/>
+      <c r="L39" s="18"/>
+      <c r="M39" s="15"/>
+      <c r="N39" s="18"/>
+      <c r="O39" s="15"/>
+      <c r="P39" s="18"/>
       <c r="Q39" s="5"/>
       <c r="R39" s="5"/>
     </row>
@@ -2104,49 +2173,49 @@
       <c r="A40" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B40" s="14" t="s">
+      <c r="B40" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="C40" s="14" t="s">
+      <c r="C40" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="D40" s="14" t="s">
+      <c r="D40" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="E40" s="14" t="s">
+      <c r="E40" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="F40" s="14" t="s">
+      <c r="F40" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="G40" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="H40" s="11" t="s">
+      <c r="G40" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="H40" s="17" t="s">
         <v>33</v>
       </c>
       <c r="K40" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L40" s="14" t="s">
+      <c r="L40" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="M40" s="14" t="s">
+      <c r="M40" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="N40" s="14" t="s">
+      <c r="N40" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="O40" s="14" t="s">
+      <c r="O40" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="P40" s="14" t="s">
+      <c r="P40" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="Q40" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="R40" s="11" t="s">
+      <c r="Q40" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="R40" s="17" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2154,23 +2223,23 @@
       <c r="A41" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B41" s="14"/>
-      <c r="C41" s="14"/>
-      <c r="D41" s="14"/>
-      <c r="E41" s="14"/>
-      <c r="F41" s="14"/>
-      <c r="G41" s="11"/>
-      <c r="H41" s="11"/>
+      <c r="B41" s="15"/>
+      <c r="C41" s="15"/>
+      <c r="D41" s="15"/>
+      <c r="E41" s="15"/>
+      <c r="F41" s="15"/>
+      <c r="G41" s="17"/>
+      <c r="H41" s="17"/>
       <c r="K41" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="L41" s="14"/>
-      <c r="M41" s="14"/>
-      <c r="N41" s="14"/>
-      <c r="O41" s="14"/>
-      <c r="P41" s="14"/>
-      <c r="Q41" s="11"/>
-      <c r="R41" s="11"/>
+      <c r="L41" s="15"/>
+      <c r="M41" s="15"/>
+      <c r="N41" s="15"/>
+      <c r="O41" s="15"/>
+      <c r="P41" s="15"/>
+      <c r="Q41" s="17"/>
+      <c r="R41" s="17"/>
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
@@ -2179,40 +2248,40 @@
       <c r="B42" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C42" s="14" t="s">
+      <c r="C42" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="D42" s="14" t="s">
+      <c r="D42" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="E42" s="14" t="s">
+      <c r="E42" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="F42" s="14" t="s">
+      <c r="F42" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="G42" s="11"/>
-      <c r="H42" s="11"/>
+      <c r="G42" s="17"/>
+      <c r="H42" s="17"/>
       <c r="K42" s="3" t="s">
         <v>22</v>
       </c>
       <c r="L42" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="M42" s="14" t="s">
+      <c r="M42" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="N42" s="14" t="s">
+      <c r="N42" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="O42" s="14" t="s">
+      <c r="O42" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="P42" s="14" t="s">
+      <c r="P42" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="Q42" s="11"/>
-      <c r="R42" s="11"/>
+      <c r="Q42" s="17"/>
+      <c r="R42" s="17"/>
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
@@ -2221,24 +2290,24 @@
       <c r="B43" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C43" s="14"/>
-      <c r="D43" s="14"/>
-      <c r="E43" s="14"/>
-      <c r="F43" s="14"/>
-      <c r="G43" s="11"/>
-      <c r="H43" s="11"/>
+      <c r="C43" s="15"/>
+      <c r="D43" s="15"/>
+      <c r="E43" s="15"/>
+      <c r="F43" s="15"/>
+      <c r="G43" s="17"/>
+      <c r="H43" s="17"/>
       <c r="K43" s="3" t="s">
         <v>21</v>
       </c>
       <c r="L43" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="M43" s="14"/>
-      <c r="N43" s="14"/>
-      <c r="O43" s="14"/>
-      <c r="P43" s="14"/>
-      <c r="Q43" s="11"/>
-      <c r="R43" s="11"/>
+      <c r="M43" s="15"/>
+      <c r="N43" s="15"/>
+      <c r="O43" s="15"/>
+      <c r="P43" s="15"/>
+      <c r="Q43" s="17"/>
+      <c r="R43" s="17"/>
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
@@ -2294,49 +2363,49 @@
       <c r="A45" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B45" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="C45" s="11" t="s">
+      <c r="B45" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="C45" s="17" t="s">
         <v>33</v>
       </c>
       <c r="D45" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="E45" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="F45" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="G45" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="H45" s="18" t="s">
+      <c r="E45" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="F45" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="G45" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="H45" s="22" t="s">
         <v>33</v>
       </c>
       <c r="K45" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="L45" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="M45" s="11" t="s">
+      <c r="L45" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="M45" s="17" t="s">
         <v>33</v>
       </c>
       <c r="N45" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="O45" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="P45" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q45" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="R45" s="18" t="s">
+      <c r="O45" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="P45" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q45" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="R45" s="22" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2344,111 +2413,111 @@
       <c r="A46" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B46" s="11"/>
-      <c r="C46" s="11"/>
-      <c r="D46" s="14" t="s">
+      <c r="B46" s="17"/>
+      <c r="C46" s="17"/>
+      <c r="D46" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="E46" s="11"/>
-      <c r="F46" s="11"/>
-      <c r="G46" s="19"/>
-      <c r="H46" s="19"/>
+      <c r="E46" s="17"/>
+      <c r="F46" s="17"/>
+      <c r="G46" s="23"/>
+      <c r="H46" s="23"/>
       <c r="K46" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="L46" s="11"/>
-      <c r="M46" s="11"/>
-      <c r="N46" s="14" t="s">
+      <c r="L46" s="17"/>
+      <c r="M46" s="17"/>
+      <c r="N46" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="O46" s="11"/>
-      <c r="P46" s="11"/>
-      <c r="Q46" s="19"/>
-      <c r="R46" s="19"/>
+      <c r="O46" s="17"/>
+      <c r="P46" s="17"/>
+      <c r="Q46" s="23"/>
+      <c r="R46" s="23"/>
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B47" s="14" t="s">
+      <c r="B47" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="C47" s="14" t="s">
+      <c r="C47" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="D47" s="14"/>
-      <c r="E47" s="11"/>
-      <c r="F47" s="14" t="s">
+      <c r="D47" s="15"/>
+      <c r="E47" s="17"/>
+      <c r="F47" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="G47" s="19"/>
-      <c r="H47" s="19"/>
+      <c r="G47" s="23"/>
+      <c r="H47" s="23"/>
       <c r="K47" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="L47" s="14" t="s">
+      <c r="L47" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="M47" s="14" t="s">
+      <c r="M47" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="N47" s="14"/>
-      <c r="O47" s="11"/>
-      <c r="P47" s="14" t="s">
+      <c r="N47" s="15"/>
+      <c r="O47" s="17"/>
+      <c r="P47" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="Q47" s="19"/>
-      <c r="R47" s="19"/>
+      <c r="Q47" s="23"/>
+      <c r="R47" s="23"/>
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B48" s="14"/>
-      <c r="C48" s="14"/>
-      <c r="D48" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="E48" s="11"/>
-      <c r="F48" s="14"/>
-      <c r="G48" s="19"/>
-      <c r="H48" s="20"/>
+      <c r="B48" s="15"/>
+      <c r="C48" s="15"/>
+      <c r="D48" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="E48" s="17"/>
+      <c r="F48" s="15"/>
+      <c r="G48" s="23"/>
+      <c r="H48" s="24"/>
       <c r="K48" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="L48" s="14"/>
-      <c r="M48" s="14"/>
-      <c r="N48" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="O48" s="11"/>
-      <c r="P48" s="14"/>
-      <c r="Q48" s="19"/>
-      <c r="R48" s="20"/>
+      <c r="L48" s="15"/>
+      <c r="M48" s="15"/>
+      <c r="N48" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="O48" s="17"/>
+      <c r="P48" s="15"/>
+      <c r="Q48" s="23"/>
+      <c r="R48" s="24"/>
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B49" s="14"/>
-      <c r="C49" s="14"/>
-      <c r="D49" s="11"/>
-      <c r="E49" s="11"/>
-      <c r="F49" s="14"/>
-      <c r="G49" s="20"/>
-      <c r="H49" s="21" t="s">
+      <c r="B49" s="15"/>
+      <c r="C49" s="15"/>
+      <c r="D49" s="17"/>
+      <c r="E49" s="17"/>
+      <c r="F49" s="15"/>
+      <c r="G49" s="24"/>
+      <c r="H49" s="25" t="s">
         <v>53</v>
       </c>
       <c r="K49" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="L49" s="14"/>
-      <c r="M49" s="14"/>
-      <c r="N49" s="11"/>
-      <c r="O49" s="11"/>
-      <c r="P49" s="14"/>
-      <c r="Q49" s="20"/>
-      <c r="R49" s="21" t="s">
+      <c r="L49" s="15"/>
+      <c r="M49" s="15"/>
+      <c r="N49" s="17"/>
+      <c r="O49" s="17"/>
+      <c r="P49" s="15"/>
+      <c r="Q49" s="24"/>
+      <c r="R49" s="25" t="s">
         <v>53</v>
       </c>
     </row>
@@ -2456,57 +2525,57 @@
       <c r="A50" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B50" s="13" t="s">
+      <c r="B50" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="C50" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="D50" s="13" t="s">
+      <c r="C50" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="D50" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="E50" s="14" t="s">
+      <c r="E50" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="F50" s="13" t="s">
+      <c r="F50" s="16" t="s">
         <v>43</v>
       </c>
       <c r="G50" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="H50" s="22"/>
+      <c r="H50" s="26"/>
       <c r="K50" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="L50" s="13" t="s">
+      <c r="L50" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="M50" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="N50" s="13" t="s">
+      <c r="M50" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="N50" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="O50" s="14" t="s">
+      <c r="O50" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="P50" s="13" t="s">
+      <c r="P50" s="16" t="s">
         <v>43</v>
       </c>
       <c r="Q50" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="R50" s="22"/>
+      <c r="R50" s="26"/>
     </row>
     <row r="51" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B51" s="13"/>
-      <c r="C51" s="12"/>
-      <c r="D51" s="13"/>
-      <c r="E51" s="14"/>
-      <c r="F51" s="13"/>
+      <c r="B51" s="16"/>
+      <c r="C51" s="18"/>
+      <c r="D51" s="16"/>
+      <c r="E51" s="15"/>
+      <c r="F51" s="16"/>
       <c r="G51" s="8" t="s">
         <v>36</v>
       </c>
@@ -2516,11 +2585,11 @@
       <c r="K51" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="L51" s="13"/>
-      <c r="M51" s="12"/>
-      <c r="N51" s="13"/>
-      <c r="O51" s="14"/>
-      <c r="P51" s="13"/>
+      <c r="L51" s="16"/>
+      <c r="M51" s="18"/>
+      <c r="N51" s="16"/>
+      <c r="O51" s="15"/>
+      <c r="P51" s="16"/>
       <c r="Q51" s="8" t="s">
         <v>81</v>
       </c>
@@ -2541,14 +2610,14 @@
       <c r="D52" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="E52" s="14"/>
+      <c r="E52" s="15"/>
       <c r="F52" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="G52" s="15" t="s">
+      <c r="G52" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="H52" s="24" t="s">
+      <c r="H52" s="11" t="s">
         <v>49</v>
       </c>
       <c r="K52" s="2" t="s">
@@ -2563,14 +2632,14 @@
       <c r="N52" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="O52" s="14"/>
+      <c r="O52" s="15"/>
       <c r="P52" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="Q52" s="15" t="s">
+      <c r="Q52" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="R52" s="16" t="s">
+      <c r="R52" s="19" t="s">
         <v>49</v>
       </c>
     </row>
@@ -2578,13 +2647,13 @@
       <c r="A53" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B53" s="16" t="s">
+      <c r="B53" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="C53" s="16" t="s">
+      <c r="C53" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="D53" s="16" t="s">
+      <c r="D53" s="19" t="s">
         <v>49</v>
       </c>
       <c r="E53" s="8" t="s">
@@ -2593,18 +2662,18 @@
       <c r="F53" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="G53" s="15"/>
-      <c r="H53" s="25"/>
+      <c r="G53" s="21"/>
+      <c r="H53" s="12"/>
       <c r="K53" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="L53" s="16" t="s">
+      <c r="L53" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="M53" s="16" t="s">
+      <c r="M53" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="N53" s="16" t="s">
+      <c r="N53" s="19" t="s">
         <v>49</v>
       </c>
       <c r="O53" s="8" t="s">
@@ -2613,42 +2682,42 @@
       <c r="P53" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="Q53" s="15"/>
-      <c r="R53" s="16"/>
+      <c r="Q53" s="21"/>
+      <c r="R53" s="19"/>
     </row>
     <row r="54" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B54" s="16"/>
-      <c r="C54" s="16"/>
-      <c r="D54" s="16"/>
+      <c r="B54" s="19"/>
+      <c r="C54" s="19"/>
+      <c r="D54" s="19"/>
       <c r="E54" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="F54" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="G54" s="17" t="s">
+      <c r="F54" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="G54" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="H54" s="26"/>
+      <c r="H54" s="13"/>
       <c r="K54" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="L54" s="16"/>
-      <c r="M54" s="16"/>
-      <c r="N54" s="16"/>
+      <c r="L54" s="19"/>
+      <c r="M54" s="19"/>
+      <c r="N54" s="19"/>
       <c r="O54" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="P54" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q54" s="17" t="s">
+      <c r="P54" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q54" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="R54" s="16"/>
+      <c r="R54" s="19"/>
     </row>
     <row r="55" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
@@ -2666,8 +2735,8 @@
       <c r="E55" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="F55" s="17"/>
-      <c r="G55" s="17"/>
+      <c r="F55" s="20"/>
+      <c r="G55" s="20"/>
       <c r="H55" s="10" t="s">
         <v>32</v>
       </c>
@@ -2686,16 +2755,175 @@
       <c r="O55" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="P55" s="17"/>
-      <c r="Q55" s="17"/>
+      <c r="P55" s="20"/>
+      <c r="Q55" s="20"/>
       <c r="R55" s="10" t="s">
         <v>32</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="188">
-    <mergeCell ref="H45:H48"/>
-    <mergeCell ref="H49:H50"/>
+  <mergeCells count="190">
+    <mergeCell ref="M50:M51"/>
+    <mergeCell ref="N50:N51"/>
+    <mergeCell ref="O50:O52"/>
+    <mergeCell ref="P50:P51"/>
+    <mergeCell ref="Q52:Q53"/>
+    <mergeCell ref="R52:R54"/>
+    <mergeCell ref="L53:L54"/>
+    <mergeCell ref="M53:M54"/>
+    <mergeCell ref="N53:N54"/>
+    <mergeCell ref="P54:P55"/>
+    <mergeCell ref="Q54:Q55"/>
+    <mergeCell ref="R40:R43"/>
+    <mergeCell ref="M42:M43"/>
+    <mergeCell ref="N42:N43"/>
+    <mergeCell ref="O42:O43"/>
+    <mergeCell ref="P42:P43"/>
+    <mergeCell ref="L45:L46"/>
+    <mergeCell ref="M45:M46"/>
+    <mergeCell ref="O45:O49"/>
+    <mergeCell ref="P45:P46"/>
+    <mergeCell ref="Q45:Q49"/>
+    <mergeCell ref="L40:L41"/>
+    <mergeCell ref="M40:M41"/>
+    <mergeCell ref="N40:N41"/>
+    <mergeCell ref="O40:O41"/>
+    <mergeCell ref="P40:P41"/>
+    <mergeCell ref="Q40:Q43"/>
+    <mergeCell ref="R45:R48"/>
+    <mergeCell ref="N46:N47"/>
+    <mergeCell ref="L47:L49"/>
+    <mergeCell ref="M47:M49"/>
+    <mergeCell ref="P47:P49"/>
+    <mergeCell ref="N48:N49"/>
+    <mergeCell ref="R49:R50"/>
+    <mergeCell ref="L50:L51"/>
+    <mergeCell ref="R32:R38"/>
+    <mergeCell ref="L38:L39"/>
+    <mergeCell ref="M38:M39"/>
+    <mergeCell ref="N38:N39"/>
+    <mergeCell ref="O38:O39"/>
+    <mergeCell ref="P38:P39"/>
+    <mergeCell ref="L32:L36"/>
+    <mergeCell ref="M32:M36"/>
+    <mergeCell ref="N32:N36"/>
+    <mergeCell ref="O32:O36"/>
+    <mergeCell ref="P32:P36"/>
+    <mergeCell ref="Q32:Q38"/>
+    <mergeCell ref="B50:B51"/>
+    <mergeCell ref="C50:C51"/>
+    <mergeCell ref="D50:D51"/>
+    <mergeCell ref="E50:E52"/>
+    <mergeCell ref="F50:F51"/>
+    <mergeCell ref="G52:G53"/>
+    <mergeCell ref="B53:B54"/>
+    <mergeCell ref="C53:C54"/>
+    <mergeCell ref="D53:D54"/>
+    <mergeCell ref="F54:F55"/>
+    <mergeCell ref="G54:G55"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="C45:C46"/>
+    <mergeCell ref="E45:E49"/>
+    <mergeCell ref="F45:F46"/>
+    <mergeCell ref="G45:G49"/>
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="C40:C41"/>
+    <mergeCell ref="D40:D41"/>
+    <mergeCell ref="E40:E41"/>
+    <mergeCell ref="F40:F41"/>
+    <mergeCell ref="G40:G43"/>
+    <mergeCell ref="D46:D47"/>
+    <mergeCell ref="B47:B49"/>
+    <mergeCell ref="C47:C49"/>
+    <mergeCell ref="F47:F49"/>
+    <mergeCell ref="D48:D49"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="C38:C39"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="E38:E39"/>
+    <mergeCell ref="F38:F39"/>
+    <mergeCell ref="B32:B36"/>
+    <mergeCell ref="C32:C36"/>
+    <mergeCell ref="D32:D36"/>
+    <mergeCell ref="E32:E36"/>
+    <mergeCell ref="F32:F36"/>
+    <mergeCell ref="R23:R25"/>
+    <mergeCell ref="L24:L25"/>
+    <mergeCell ref="M24:M25"/>
+    <mergeCell ref="N24:N25"/>
+    <mergeCell ref="P25:P26"/>
+    <mergeCell ref="Q25:Q26"/>
+    <mergeCell ref="L21:L22"/>
+    <mergeCell ref="M21:M22"/>
+    <mergeCell ref="N21:N22"/>
+    <mergeCell ref="O21:O23"/>
+    <mergeCell ref="P21:P22"/>
+    <mergeCell ref="Q23:Q24"/>
+    <mergeCell ref="N19:N20"/>
+    <mergeCell ref="M11:M12"/>
+    <mergeCell ref="N11:N12"/>
+    <mergeCell ref="O11:O12"/>
+    <mergeCell ref="P11:P12"/>
+    <mergeCell ref="Q11:Q14"/>
+    <mergeCell ref="R11:R14"/>
+    <mergeCell ref="M13:M14"/>
+    <mergeCell ref="N13:N14"/>
+    <mergeCell ref="O13:O14"/>
+    <mergeCell ref="P13:P14"/>
+    <mergeCell ref="Q16:Q20"/>
+    <mergeCell ref="R16:R19"/>
+    <mergeCell ref="R20:R21"/>
+    <mergeCell ref="M16:M17"/>
+    <mergeCell ref="O16:O20"/>
+    <mergeCell ref="P16:P17"/>
+    <mergeCell ref="N17:N18"/>
+    <mergeCell ref="M18:M20"/>
+    <mergeCell ref="P18:P20"/>
+    <mergeCell ref="M3:M7"/>
+    <mergeCell ref="N3:N7"/>
+    <mergeCell ref="O3:O7"/>
+    <mergeCell ref="P3:P7"/>
+    <mergeCell ref="Q3:Q9"/>
+    <mergeCell ref="R3:R9"/>
+    <mergeCell ref="M9:M10"/>
+    <mergeCell ref="N9:N10"/>
+    <mergeCell ref="O9:O10"/>
+    <mergeCell ref="P9:P10"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="G23:G24"/>
+    <mergeCell ref="G25:G26"/>
+    <mergeCell ref="H23:H25"/>
+    <mergeCell ref="L3:L7"/>
+    <mergeCell ref="L9:L10"/>
+    <mergeCell ref="L11:L12"/>
+    <mergeCell ref="L16:L17"/>
+    <mergeCell ref="L18:L20"/>
+    <mergeCell ref="F16:F17"/>
+    <mergeCell ref="H16:H19"/>
+    <mergeCell ref="H20:H21"/>
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="G10:G11"/>
+    <mergeCell ref="G3:G8"/>
+    <mergeCell ref="H3:H8"/>
+    <mergeCell ref="H10:H14"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="C18:C20"/>
+    <mergeCell ref="F18:F20"/>
+    <mergeCell ref="E21:E23"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="B3:B7"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E16:E20"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="D9:D10"/>
     <mergeCell ref="F9:F10"/>
     <mergeCell ref="C9:C10"/>
     <mergeCell ref="D11:D12"/>
@@ -2720,168 +2948,11 @@
     <mergeCell ref="H40:H43"/>
     <mergeCell ref="C42:C43"/>
     <mergeCell ref="D42:D43"/>
-    <mergeCell ref="B3:B7"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="E16:E20"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="G23:G24"/>
-    <mergeCell ref="G25:G26"/>
-    <mergeCell ref="H23:H25"/>
-    <mergeCell ref="L3:L7"/>
-    <mergeCell ref="L9:L10"/>
-    <mergeCell ref="L11:L12"/>
-    <mergeCell ref="L16:L17"/>
-    <mergeCell ref="L18:L20"/>
-    <mergeCell ref="F16:F17"/>
-    <mergeCell ref="G11:G14"/>
-    <mergeCell ref="H11:H14"/>
-    <mergeCell ref="G3:G9"/>
-    <mergeCell ref="H3:H9"/>
-    <mergeCell ref="H16:H19"/>
-    <mergeCell ref="H20:H21"/>
-    <mergeCell ref="G16:G20"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="F21:F22"/>
-    <mergeCell ref="C18:C20"/>
-    <mergeCell ref="F18:F20"/>
-    <mergeCell ref="E21:E23"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="M3:M7"/>
-    <mergeCell ref="N3:N7"/>
-    <mergeCell ref="O3:O7"/>
-    <mergeCell ref="P3:P7"/>
-    <mergeCell ref="Q3:Q9"/>
-    <mergeCell ref="R3:R9"/>
-    <mergeCell ref="M9:M10"/>
-    <mergeCell ref="N9:N10"/>
-    <mergeCell ref="O9:O10"/>
-    <mergeCell ref="P9:P10"/>
-    <mergeCell ref="N19:N20"/>
-    <mergeCell ref="M11:M12"/>
-    <mergeCell ref="N11:N12"/>
-    <mergeCell ref="O11:O12"/>
-    <mergeCell ref="P11:P12"/>
-    <mergeCell ref="Q11:Q14"/>
-    <mergeCell ref="R11:R14"/>
-    <mergeCell ref="M13:M14"/>
-    <mergeCell ref="N13:N14"/>
-    <mergeCell ref="O13:O14"/>
-    <mergeCell ref="P13:P14"/>
-    <mergeCell ref="Q16:Q20"/>
-    <mergeCell ref="R16:R19"/>
-    <mergeCell ref="R20:R21"/>
-    <mergeCell ref="M16:M17"/>
-    <mergeCell ref="O16:O20"/>
-    <mergeCell ref="P16:P17"/>
-    <mergeCell ref="N17:N18"/>
-    <mergeCell ref="M18:M20"/>
-    <mergeCell ref="P18:P20"/>
-    <mergeCell ref="R23:R25"/>
-    <mergeCell ref="L24:L25"/>
-    <mergeCell ref="M24:M25"/>
-    <mergeCell ref="N24:N25"/>
-    <mergeCell ref="P25:P26"/>
-    <mergeCell ref="Q25:Q26"/>
-    <mergeCell ref="L21:L22"/>
-    <mergeCell ref="M21:M22"/>
-    <mergeCell ref="N21:N22"/>
-    <mergeCell ref="O21:O23"/>
-    <mergeCell ref="P21:P22"/>
-    <mergeCell ref="Q23:Q24"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="C38:C39"/>
-    <mergeCell ref="D38:D39"/>
-    <mergeCell ref="E38:E39"/>
-    <mergeCell ref="F38:F39"/>
-    <mergeCell ref="B32:B36"/>
-    <mergeCell ref="C32:C36"/>
-    <mergeCell ref="D32:D36"/>
-    <mergeCell ref="E32:E36"/>
-    <mergeCell ref="F32:F36"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="C45:C46"/>
-    <mergeCell ref="E45:E49"/>
-    <mergeCell ref="F45:F46"/>
-    <mergeCell ref="G45:G49"/>
-    <mergeCell ref="B40:B41"/>
-    <mergeCell ref="C40:C41"/>
-    <mergeCell ref="D40:D41"/>
-    <mergeCell ref="E40:E41"/>
-    <mergeCell ref="F40:F41"/>
-    <mergeCell ref="G40:G43"/>
-    <mergeCell ref="D46:D47"/>
-    <mergeCell ref="B47:B49"/>
-    <mergeCell ref="C47:C49"/>
-    <mergeCell ref="F47:F49"/>
-    <mergeCell ref="D48:D49"/>
     <mergeCell ref="E42:E43"/>
     <mergeCell ref="F42:F43"/>
-    <mergeCell ref="B50:B51"/>
-    <mergeCell ref="C50:C51"/>
-    <mergeCell ref="D50:D51"/>
-    <mergeCell ref="E50:E52"/>
-    <mergeCell ref="F50:F51"/>
-    <mergeCell ref="G52:G53"/>
-    <mergeCell ref="B53:B54"/>
-    <mergeCell ref="C53:C54"/>
-    <mergeCell ref="D53:D54"/>
-    <mergeCell ref="F54:F55"/>
-    <mergeCell ref="G54:G55"/>
-    <mergeCell ref="R32:R38"/>
-    <mergeCell ref="L38:L39"/>
-    <mergeCell ref="M38:M39"/>
-    <mergeCell ref="N38:N39"/>
-    <mergeCell ref="O38:O39"/>
-    <mergeCell ref="P38:P39"/>
-    <mergeCell ref="L32:L36"/>
-    <mergeCell ref="M32:M36"/>
-    <mergeCell ref="N32:N36"/>
-    <mergeCell ref="O32:O36"/>
-    <mergeCell ref="P32:P36"/>
-    <mergeCell ref="Q32:Q38"/>
-    <mergeCell ref="R40:R43"/>
-    <mergeCell ref="M42:M43"/>
-    <mergeCell ref="N42:N43"/>
-    <mergeCell ref="O42:O43"/>
-    <mergeCell ref="P42:P43"/>
-    <mergeCell ref="L45:L46"/>
-    <mergeCell ref="M45:M46"/>
-    <mergeCell ref="O45:O49"/>
-    <mergeCell ref="P45:P46"/>
-    <mergeCell ref="Q45:Q49"/>
-    <mergeCell ref="L40:L41"/>
-    <mergeCell ref="M40:M41"/>
-    <mergeCell ref="N40:N41"/>
-    <mergeCell ref="O40:O41"/>
-    <mergeCell ref="P40:P41"/>
-    <mergeCell ref="Q40:Q43"/>
-    <mergeCell ref="R45:R48"/>
-    <mergeCell ref="N46:N47"/>
-    <mergeCell ref="L47:L49"/>
-    <mergeCell ref="M47:M49"/>
-    <mergeCell ref="P47:P49"/>
-    <mergeCell ref="N48:N49"/>
-    <mergeCell ref="R49:R50"/>
-    <mergeCell ref="L50:L51"/>
-    <mergeCell ref="M50:M51"/>
-    <mergeCell ref="N50:N51"/>
-    <mergeCell ref="O50:O52"/>
-    <mergeCell ref="P50:P51"/>
-    <mergeCell ref="Q52:Q53"/>
-    <mergeCell ref="R52:R54"/>
-    <mergeCell ref="L53:L54"/>
-    <mergeCell ref="M53:M54"/>
-    <mergeCell ref="N53:N54"/>
-    <mergeCell ref="P54:P55"/>
-    <mergeCell ref="Q54:Q55"/>
+    <mergeCell ref="H45:H48"/>
+    <mergeCell ref="H49:H50"/>
+    <mergeCell ref="G18:G21"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Cambio de actividades semana 20 a 24 de febrero
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MATEO\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MATEO\Desktop\Platzi\Curso Git - GutHub\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D79D9D44-1D2A-4613-8931-82F30E1807D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6015A316-79E4-44BB-B606-5D7445FB224F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{A899F46E-BA08-4AC6-A7C3-F03724044CD5}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="91">
   <si>
     <t>Hora</t>
   </si>
@@ -300,13 +300,22 @@
   </si>
   <si>
     <t>Compras - Cena</t>
+  </si>
+  <si>
+    <t>Estudio de Eagle</t>
+  </si>
+  <si>
+    <t>Reunion lab control</t>
+  </si>
+  <si>
+    <t>Estudio digital y practica</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -326,6 +335,12 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Baguet Script"/>
+    </font>
+    <font>
+      <u/>
       <sz val="9"/>
       <color theme="1"/>
       <name val="Baguet Script"/>
@@ -445,7 +460,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -475,37 +490,25 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -523,6 +526,9 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -530,6 +536,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -848,8 +866,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9132D586-DE4C-4B7E-830E-683E06A9C036}">
   <dimension ref="A2:R55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="117" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12:G13"/>
+    <sheetView tabSelected="1" topLeftCell="L3" zoomScale="117" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q22" sqref="Q22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -929,25 +947,25 @@
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="C3" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="D3" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="E3" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="F3" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="G3" s="27" t="s">
-        <v>32</v>
-      </c>
-      <c r="H3" s="27" t="s">
+      <c r="B3" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="G3" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="H3" s="24" t="s">
         <v>32</v>
       </c>
       <c r="I3" s="2" t="s">
@@ -957,25 +975,25 @@
       <c r="K3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="L3" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="M3" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="N3" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="O3" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="P3" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q3" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="R3" s="14" t="s">
+      <c r="L3" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="M3" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="N3" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="O3" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="P3" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q3" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="R3" s="23" t="s">
         <v>32</v>
       </c>
     </row>
@@ -983,13 +1001,13 @@
       <c r="A4" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="28"/>
-      <c r="H4" s="28"/>
+      <c r="B4" s="23"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="25"/>
       <c r="I4" s="3" t="s">
         <v>31</v>
       </c>
@@ -997,25 +1015,25 @@
       <c r="K4" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="L4" s="14"/>
-      <c r="M4" s="14"/>
-      <c r="N4" s="14"/>
-      <c r="O4" s="14"/>
-      <c r="P4" s="14"/>
-      <c r="Q4" s="14"/>
-      <c r="R4" s="14"/>
+      <c r="L4" s="23"/>
+      <c r="M4" s="23"/>
+      <c r="N4" s="23"/>
+      <c r="O4" s="23"/>
+      <c r="P4" s="23"/>
+      <c r="Q4" s="23"/>
+      <c r="R4" s="23"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="14"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="28"/>
-      <c r="H5" s="28"/>
+      <c r="B5" s="23"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="25"/>
+      <c r="H5" s="25"/>
       <c r="I5" s="3" t="s">
         <v>30</v>
       </c>
@@ -1023,25 +1041,25 @@
       <c r="K5" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="L5" s="14"/>
-      <c r="M5" s="14"/>
-      <c r="N5" s="14"/>
-      <c r="O5" s="14"/>
-      <c r="P5" s="14"/>
-      <c r="Q5" s="14"/>
-      <c r="R5" s="14"/>
+      <c r="L5" s="23"/>
+      <c r="M5" s="23"/>
+      <c r="N5" s="23"/>
+      <c r="O5" s="23"/>
+      <c r="P5" s="23"/>
+      <c r="Q5" s="23"/>
+      <c r="R5" s="23"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B6" s="14"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="28"/>
-      <c r="H6" s="28"/>
+      <c r="B6" s="23"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="25"/>
+      <c r="H6" s="25"/>
       <c r="I6" s="3" t="s">
         <v>29</v>
       </c>
@@ -1049,25 +1067,25 @@
       <c r="K6" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="L6" s="14"/>
-      <c r="M6" s="14"/>
-      <c r="N6" s="14"/>
-      <c r="O6" s="14"/>
-      <c r="P6" s="14"/>
-      <c r="Q6" s="14"/>
-      <c r="R6" s="14"/>
+      <c r="L6" s="23"/>
+      <c r="M6" s="23"/>
+      <c r="N6" s="23"/>
+      <c r="O6" s="23"/>
+      <c r="P6" s="23"/>
+      <c r="Q6" s="23"/>
+      <c r="R6" s="23"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="14"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="28"/>
-      <c r="H7" s="28"/>
+      <c r="B7" s="23"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="25"/>
+      <c r="H7" s="25"/>
       <c r="I7" s="3" t="s">
         <v>28</v>
       </c>
@@ -1075,13 +1093,13 @@
       <c r="K7" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="L7" s="14"/>
-      <c r="M7" s="14"/>
-      <c r="N7" s="14"/>
-      <c r="O7" s="14"/>
-      <c r="P7" s="14"/>
-      <c r="Q7" s="14"/>
-      <c r="R7" s="14"/>
+      <c r="L7" s="23"/>
+      <c r="M7" s="23"/>
+      <c r="N7" s="23"/>
+      <c r="O7" s="23"/>
+      <c r="P7" s="23"/>
+      <c r="Q7" s="23"/>
+      <c r="R7" s="23"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
@@ -1092,8 +1110,8 @@
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
-      <c r="G8" s="29"/>
-      <c r="H8" s="29"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="26"/>
       <c r="I8" s="3" t="s">
         <v>27</v>
       </c>
@@ -1106,26 +1124,26 @@
       <c r="N8" s="5"/>
       <c r="O8" s="5"/>
       <c r="P8" s="5"/>
-      <c r="Q8" s="14"/>
-      <c r="R8" s="14"/>
+      <c r="Q8" s="23"/>
+      <c r="R8" s="23"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="C9" s="15" t="s">
+      <c r="B9" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="D9" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="E9" s="15" t="s">
+      <c r="D9" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="F9" s="17" t="s">
+      <c r="F9" s="11" t="s">
         <v>33</v>
       </c>
       <c r="G9" s="5"/>
@@ -1137,37 +1155,37 @@
       <c r="K9" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="L9" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="M9" s="15" t="s">
+      <c r="L9" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="M9" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="N9" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="O9" s="15" t="s">
+      <c r="N9" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="O9" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="P9" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q9" s="14"/>
-      <c r="R9" s="14"/>
+      <c r="P9" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q9" s="23"/>
+      <c r="R9" s="23"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="18"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="22" t="s">
+      <c r="B10" s="12"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="H10" s="22" t="s">
+      <c r="H10" s="18" t="s">
         <v>33</v>
       </c>
       <c r="I10" s="3" t="s">
@@ -1177,11 +1195,11 @@
       <c r="K10" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="L10" s="18"/>
-      <c r="M10" s="15"/>
-      <c r="N10" s="18"/>
-      <c r="O10" s="15"/>
-      <c r="P10" s="18"/>
+      <c r="L10" s="12"/>
+      <c r="M10" s="14"/>
+      <c r="N10" s="12"/>
+      <c r="O10" s="14"/>
+      <c r="P10" s="12"/>
       <c r="Q10" s="5"/>
       <c r="R10" s="5"/>
     </row>
@@ -1189,23 +1207,23 @@
       <c r="A11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="C11" s="15" t="s">
+      <c r="C11" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="D11" s="15" t="s">
+      <c r="D11" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="E11" s="15" t="s">
+      <c r="E11" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="F11" s="15" t="s">
+      <c r="F11" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="G11" s="24"/>
-      <c r="H11" s="23"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="19"/>
       <c r="I11" s="3" t="s">
         <v>24</v>
       </c>
@@ -1213,25 +1231,25 @@
       <c r="K11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L11" s="15" t="s">
+      <c r="L11" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="M11" s="15" t="s">
+      <c r="M11" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="N11" s="15" t="s">
+      <c r="N11" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="O11" s="15" t="s">
+      <c r="O11" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="P11" s="15" t="s">
+      <c r="P11" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="Q11" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="R11" s="17" t="s">
+      <c r="Q11" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="R11" s="11" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1239,15 +1257,15 @@
       <c r="A12" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="15"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="16" t="s">
+      <c r="B12" s="14"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="H12" s="23"/>
+      <c r="H12" s="19"/>
       <c r="I12" s="3" t="s">
         <v>23</v>
       </c>
@@ -1255,13 +1273,13 @@
       <c r="K12" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="L12" s="15"/>
-      <c r="M12" s="15"/>
-      <c r="N12" s="15"/>
-      <c r="O12" s="15"/>
-      <c r="P12" s="15"/>
-      <c r="Q12" s="17"/>
-      <c r="R12" s="17"/>
+      <c r="L12" s="14"/>
+      <c r="M12" s="14"/>
+      <c r="N12" s="14"/>
+      <c r="O12" s="14"/>
+      <c r="P12" s="14"/>
+      <c r="Q12" s="11"/>
+      <c r="R12" s="11"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
@@ -1270,20 +1288,20 @@
       <c r="B13" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C13" s="15" t="s">
+      <c r="C13" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="D13" s="15" t="s">
+      <c r="D13" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="E13" s="15" t="s">
+      <c r="E13" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="F13" s="15" t="s">
+      <c r="F13" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="G13" s="16"/>
-      <c r="H13" s="23"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="19"/>
       <c r="I13" s="3" t="s">
         <v>22</v>
       </c>
@@ -1294,20 +1312,20 @@
       <c r="L13" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="M13" s="15" t="s">
+      <c r="M13" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="N13" s="15" t="s">
+      <c r="N13" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="O13" s="15" t="s">
+      <c r="O13" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="P13" s="15" t="s">
+      <c r="P13" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="Q13" s="17"/>
-      <c r="R13" s="17"/>
+      <c r="Q13" s="11"/>
+      <c r="R13" s="11"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
@@ -1316,14 +1334,14 @@
       <c r="B14" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="15"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
       <c r="G14" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="H14" s="24"/>
+      <c r="H14" s="20"/>
       <c r="I14" s="3" t="s">
         <v>21</v>
       </c>
@@ -1334,12 +1352,12 @@
       <c r="L14" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="M14" s="15"/>
-      <c r="N14" s="15"/>
-      <c r="O14" s="15"/>
-      <c r="P14" s="15"/>
-      <c r="Q14" s="17"/>
-      <c r="R14" s="17"/>
+      <c r="M14" s="14"/>
+      <c r="N14" s="14"/>
+      <c r="O14" s="14"/>
+      <c r="P14" s="14"/>
+      <c r="Q14" s="11"/>
+      <c r="R14" s="11"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
@@ -1399,25 +1417,25 @@
       <c r="A16" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="C16" s="17" t="s">
+      <c r="B16" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="11" t="s">
         <v>33</v>
       </c>
       <c r="D16" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="E16" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="F16" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="G16" s="22" t="s">
+      <c r="E16" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="G16" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="H16" s="22" t="s">
+      <c r="H16" s="18" t="s">
         <v>33</v>
       </c>
       <c r="I16" s="3" t="s">
@@ -1427,25 +1445,25 @@
       <c r="K16" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="L16" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="M16" s="17" t="s">
+      <c r="L16" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="M16" s="11" t="s">
         <v>33</v>
       </c>
       <c r="N16" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="O16" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="P16" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q16" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="R16" s="22" t="s">
+        <v>89</v>
+      </c>
+      <c r="O16" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="P16" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q16" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="R16" s="18" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1453,15 +1471,15 @@
       <c r="A17" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="17"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="15" t="s">
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="E17" s="17"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="23"/>
-      <c r="H17" s="23"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="19"/>
+      <c r="H17" s="19"/>
       <c r="I17" s="3" t="s">
         <v>19</v>
       </c>
@@ -1469,35 +1487,35 @@
       <c r="K17" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="L17" s="17"/>
-      <c r="M17" s="17"/>
-      <c r="N17" s="15" t="s">
+      <c r="L17" s="11"/>
+      <c r="M17" s="11"/>
+      <c r="N17" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="O17" s="17"/>
-      <c r="P17" s="17"/>
-      <c r="Q17" s="23"/>
-      <c r="R17" s="23"/>
+      <c r="O17" s="11"/>
+      <c r="P17" s="11"/>
+      <c r="Q17" s="19"/>
+      <c r="R17" s="19"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="15" t="s">
+      <c r="B18" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="C18" s="15" t="s">
+      <c r="C18" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="D18" s="15"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="15" t="s">
+      <c r="D18" s="14"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="G18" s="22" t="s">
+      <c r="G18" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="H18" s="23"/>
+      <c r="H18" s="19"/>
       <c r="I18" s="3" t="s">
         <v>17</v>
       </c>
@@ -1505,33 +1523,33 @@
       <c r="K18" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="L18" s="15" t="s">
+      <c r="L18" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="M18" s="15" t="s">
+      <c r="M18" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="N18" s="15"/>
-      <c r="O18" s="17"/>
-      <c r="P18" s="15" t="s">
+      <c r="N18" s="14"/>
+      <c r="O18" s="11"/>
+      <c r="P18" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="Q18" s="23"/>
-      <c r="R18" s="23"/>
+      <c r="Q18" s="19"/>
+      <c r="R18" s="19"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="15"/>
-      <c r="C19" s="15"/>
-      <c r="D19" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="E19" s="17"/>
-      <c r="F19" s="15"/>
-      <c r="G19" s="23"/>
-      <c r="H19" s="24"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E19" s="11"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="19"/>
+      <c r="H19" s="20"/>
       <c r="I19" s="3" t="s">
         <v>16</v>
       </c>
@@ -1539,27 +1557,27 @@
       <c r="K19" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="L19" s="15"/>
-      <c r="M19" s="15"/>
-      <c r="N19" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="O19" s="17"/>
-      <c r="P19" s="15"/>
-      <c r="Q19" s="23"/>
-      <c r="R19" s="24"/>
+      <c r="L19" s="14"/>
+      <c r="M19" s="14"/>
+      <c r="N19" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="O19" s="11"/>
+      <c r="P19" s="14"/>
+      <c r="Q19" s="19"/>
+      <c r="R19" s="20"/>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="15"/>
-      <c r="C20" s="15"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="15"/>
-      <c r="G20" s="23"/>
-      <c r="H20" s="25" t="s">
+      <c r="B20" s="14"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="19"/>
+      <c r="H20" s="21" t="s">
         <v>53</v>
       </c>
       <c r="I20" s="3" t="s">
@@ -1569,13 +1587,13 @@
       <c r="K20" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="L20" s="15"/>
-      <c r="M20" s="15"/>
-      <c r="N20" s="17"/>
-      <c r="O20" s="17"/>
-      <c r="P20" s="15"/>
-      <c r="Q20" s="24"/>
-      <c r="R20" s="25" t="s">
+      <c r="L20" s="14"/>
+      <c r="M20" s="14"/>
+      <c r="N20" s="19"/>
+      <c r="O20" s="11"/>
+      <c r="P20" s="14"/>
+      <c r="Q20" s="20"/>
+      <c r="R20" s="21" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1583,23 +1601,23 @@
       <c r="A21" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B21" s="16" t="s">
+      <c r="B21" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="C21" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="D21" s="16" t="s">
+      <c r="C21" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D21" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="E21" s="15" t="s">
+      <c r="E21" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="F21" s="16" t="s">
+      <c r="F21" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="G21" s="24"/>
-      <c r="H21" s="26"/>
+      <c r="G21" s="20"/>
+      <c r="H21" s="22"/>
       <c r="I21" s="3" t="s">
         <v>15</v>
       </c>
@@ -1607,35 +1625,33 @@
       <c r="K21" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="L21" s="16" t="s">
+      <c r="L21" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="M21" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="N21" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="O21" s="15" t="s">
+      <c r="M21" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="N21" s="19"/>
+      <c r="O21" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="P21" s="16" t="s">
+      <c r="P21" s="30" t="s">
         <v>43</v>
       </c>
       <c r="Q21" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="R21" s="26"/>
+      <c r="R21" s="22"/>
     </row>
     <row r="22" spans="1:18" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B22" s="16"/>
-      <c r="C22" s="18"/>
-      <c r="D22" s="16"/>
-      <c r="E22" s="15"/>
-      <c r="F22" s="16"/>
+      <c r="B22" s="13"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="13"/>
       <c r="G22" s="8" t="s">
         <v>87</v>
       </c>
@@ -1649,11 +1665,11 @@
       <c r="K22" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="L22" s="16"/>
-      <c r="M22" s="18"/>
-      <c r="N22" s="16"/>
-      <c r="O22" s="15"/>
-      <c r="P22" s="16"/>
+      <c r="L22" s="13"/>
+      <c r="M22" s="12"/>
+      <c r="N22" s="20"/>
+      <c r="O22" s="14"/>
+      <c r="P22" s="30"/>
       <c r="Q22" s="8" t="s">
         <v>77</v>
       </c>
@@ -1674,14 +1690,14 @@
       <c r="D23" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="E23" s="15"/>
+      <c r="E23" s="14"/>
       <c r="F23" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="G23" s="17" t="s">
+      <c r="G23" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="H23" s="19" t="s">
+      <c r="H23" s="16" t="s">
         <v>49</v>
       </c>
       <c r="I23" s="2" t="s">
@@ -1700,14 +1716,14 @@
       <c r="N23" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="O23" s="15"/>
+      <c r="O23" s="14"/>
       <c r="P23" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="Q23" s="21" t="s">
+      <c r="Q23" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="R23" s="19" t="s">
+      <c r="R23" s="16" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1715,13 +1731,13 @@
       <c r="A24" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B24" s="19" t="s">
+      <c r="B24" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="C24" s="19" t="s">
+      <c r="C24" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="D24" s="19" t="s">
+      <c r="D24" s="16" t="s">
         <v>49</v>
       </c>
       <c r="E24" s="8" t="s">
@@ -1730,8 +1746,8 @@
       <c r="F24" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="G24" s="17"/>
-      <c r="H24" s="19"/>
+      <c r="G24" s="11"/>
+      <c r="H24" s="16"/>
       <c r="I24" s="2" t="s">
         <v>11</v>
       </c>
@@ -1739,13 +1755,13 @@
       <c r="K24" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="L24" s="19" t="s">
+      <c r="L24" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="M24" s="19" t="s">
+      <c r="M24" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="N24" s="19" t="s">
+      <c r="N24" s="16" t="s">
         <v>49</v>
       </c>
       <c r="O24" s="8" t="s">
@@ -1754,26 +1770,26 @@
       <c r="P24" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="Q24" s="21"/>
-      <c r="R24" s="19"/>
+      <c r="Q24" s="15"/>
+      <c r="R24" s="16"/>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B25" s="19"/>
-      <c r="C25" s="19"/>
-      <c r="D25" s="19"/>
+      <c r="B25" s="16"/>
+      <c r="C25" s="16"/>
+      <c r="D25" s="16"/>
       <c r="E25" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="F25" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="G25" s="20" t="s">
+      <c r="F25" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="G25" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="H25" s="19"/>
+      <c r="H25" s="16"/>
       <c r="I25" s="2" t="s">
         <v>12</v>
       </c>
@@ -1781,19 +1797,19 @@
       <c r="K25" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="L25" s="19"/>
-      <c r="M25" s="19"/>
-      <c r="N25" s="19"/>
+      <c r="L25" s="16"/>
+      <c r="M25" s="16"/>
+      <c r="N25" s="16"/>
       <c r="O25" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="P25" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q25" s="20" t="s">
+      <c r="P25" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q25" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="R25" s="19"/>
+      <c r="R25" s="16"/>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
@@ -1811,8 +1827,8 @@
       <c r="E26" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="F26" s="20"/>
-      <c r="G26" s="20"/>
+      <c r="F26" s="17"/>
+      <c r="G26" s="17"/>
       <c r="H26" s="10" t="s">
         <v>32</v>
       </c>
@@ -1835,8 +1851,8 @@
       <c r="O26" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="P26" s="20"/>
-      <c r="Q26" s="20"/>
+      <c r="P26" s="17"/>
+      <c r="Q26" s="17"/>
       <c r="R26" s="10" t="s">
         <v>32</v>
       </c>
@@ -1949,49 +1965,49 @@
       <c r="A32" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B32" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="C32" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="D32" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="E32" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="F32" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="G32" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="H32" s="14" t="s">
+      <c r="B32" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="C32" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="D32" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="E32" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="F32" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="G32" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="H32" s="23" t="s">
         <v>32</v>
       </c>
       <c r="K32" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="L32" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="M32" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="N32" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="O32" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="P32" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q32" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="R32" s="14" t="s">
+      <c r="L32" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="M32" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="N32" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="O32" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="P32" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q32" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="R32" s="23" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1999,89 +2015,89 @@
       <c r="A33" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B33" s="14"/>
-      <c r="C33" s="14"/>
-      <c r="D33" s="14"/>
-      <c r="E33" s="14"/>
-      <c r="F33" s="14"/>
-      <c r="G33" s="14"/>
-      <c r="H33" s="14"/>
+      <c r="B33" s="23"/>
+      <c r="C33" s="23"/>
+      <c r="D33" s="23"/>
+      <c r="E33" s="23"/>
+      <c r="F33" s="23"/>
+      <c r="G33" s="23"/>
+      <c r="H33" s="23"/>
       <c r="K33" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="L33" s="14"/>
-      <c r="M33" s="14"/>
-      <c r="N33" s="14"/>
-      <c r="O33" s="14"/>
-      <c r="P33" s="14"/>
-      <c r="Q33" s="14"/>
-      <c r="R33" s="14"/>
+      <c r="L33" s="23"/>
+      <c r="M33" s="23"/>
+      <c r="N33" s="23"/>
+      <c r="O33" s="23"/>
+      <c r="P33" s="23"/>
+      <c r="Q33" s="23"/>
+      <c r="R33" s="23"/>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B34" s="14"/>
-      <c r="C34" s="14"/>
-      <c r="D34" s="14"/>
-      <c r="E34" s="14"/>
-      <c r="F34" s="14"/>
-      <c r="G34" s="14"/>
-      <c r="H34" s="14"/>
+      <c r="B34" s="23"/>
+      <c r="C34" s="23"/>
+      <c r="D34" s="23"/>
+      <c r="E34" s="23"/>
+      <c r="F34" s="23"/>
+      <c r="G34" s="23"/>
+      <c r="H34" s="23"/>
       <c r="K34" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="L34" s="14"/>
-      <c r="M34" s="14"/>
-      <c r="N34" s="14"/>
-      <c r="O34" s="14"/>
-      <c r="P34" s="14"/>
-      <c r="Q34" s="14"/>
-      <c r="R34" s="14"/>
+      <c r="L34" s="23"/>
+      <c r="M34" s="23"/>
+      <c r="N34" s="23"/>
+      <c r="O34" s="23"/>
+      <c r="P34" s="23"/>
+      <c r="Q34" s="23"/>
+      <c r="R34" s="23"/>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B35" s="14"/>
-      <c r="C35" s="14"/>
-      <c r="D35" s="14"/>
-      <c r="E35" s="14"/>
-      <c r="F35" s="14"/>
-      <c r="G35" s="14"/>
-      <c r="H35" s="14"/>
+      <c r="B35" s="23"/>
+      <c r="C35" s="23"/>
+      <c r="D35" s="23"/>
+      <c r="E35" s="23"/>
+      <c r="F35" s="23"/>
+      <c r="G35" s="23"/>
+      <c r="H35" s="23"/>
       <c r="K35" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="L35" s="14"/>
-      <c r="M35" s="14"/>
-      <c r="N35" s="14"/>
-      <c r="O35" s="14"/>
-      <c r="P35" s="14"/>
-      <c r="Q35" s="14"/>
-      <c r="R35" s="14"/>
+      <c r="L35" s="23"/>
+      <c r="M35" s="23"/>
+      <c r="N35" s="23"/>
+      <c r="O35" s="23"/>
+      <c r="P35" s="23"/>
+      <c r="Q35" s="23"/>
+      <c r="R35" s="23"/>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B36" s="14"/>
-      <c r="C36" s="14"/>
-      <c r="D36" s="14"/>
-      <c r="E36" s="14"/>
-      <c r="F36" s="14"/>
-      <c r="G36" s="14"/>
-      <c r="H36" s="14"/>
+      <c r="B36" s="23"/>
+      <c r="C36" s="23"/>
+      <c r="D36" s="23"/>
+      <c r="E36" s="23"/>
+      <c r="F36" s="23"/>
+      <c r="G36" s="23"/>
+      <c r="H36" s="23"/>
       <c r="K36" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="L36" s="14"/>
-      <c r="M36" s="14"/>
-      <c r="N36" s="14"/>
-      <c r="O36" s="14"/>
-      <c r="P36" s="14"/>
-      <c r="Q36" s="14"/>
-      <c r="R36" s="14"/>
+      <c r="L36" s="23"/>
+      <c r="M36" s="23"/>
+      <c r="N36" s="23"/>
+      <c r="O36" s="23"/>
+      <c r="P36" s="23"/>
+      <c r="Q36" s="23"/>
+      <c r="R36" s="23"/>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
@@ -2092,8 +2108,8 @@
       <c r="D37" s="5"/>
       <c r="E37" s="5"/>
       <c r="F37" s="5"/>
-      <c r="G37" s="14"/>
-      <c r="H37" s="14"/>
+      <c r="G37" s="23"/>
+      <c r="H37" s="23"/>
       <c r="K37" s="3" t="s">
         <v>27</v>
       </c>
@@ -2102,70 +2118,70 @@
       <c r="N37" s="5"/>
       <c r="O37" s="5"/>
       <c r="P37" s="5"/>
-      <c r="Q37" s="14"/>
-      <c r="R37" s="14"/>
+      <c r="Q37" s="23"/>
+      <c r="R37" s="23"/>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B38" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="C38" s="15" t="s">
+      <c r="B38" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C38" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="D38" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="E38" s="15" t="s">
+      <c r="D38" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E38" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="F38" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="G38" s="14"/>
-      <c r="H38" s="14"/>
+      <c r="F38" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="G38" s="23"/>
+      <c r="H38" s="23"/>
       <c r="K38" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="L38" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="M38" s="15" t="s">
+      <c r="L38" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="M38" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="N38" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="O38" s="15" t="s">
+      <c r="N38" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="O38" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="P38" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q38" s="14"/>
-      <c r="R38" s="14"/>
+      <c r="P38" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q38" s="23"/>
+      <c r="R38" s="23"/>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B39" s="18"/>
-      <c r="C39" s="15"/>
-      <c r="D39" s="18"/>
-      <c r="E39" s="15"/>
-      <c r="F39" s="18"/>
+      <c r="B39" s="12"/>
+      <c r="C39" s="14"/>
+      <c r="D39" s="12"/>
+      <c r="E39" s="14"/>
+      <c r="F39" s="12"/>
       <c r="G39" s="5"/>
       <c r="H39" s="5"/>
       <c r="K39" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="L39" s="18"/>
-      <c r="M39" s="15"/>
-      <c r="N39" s="18"/>
-      <c r="O39" s="15"/>
-      <c r="P39" s="18"/>
+      <c r="L39" s="12"/>
+      <c r="M39" s="14"/>
+      <c r="N39" s="12"/>
+      <c r="O39" s="14"/>
+      <c r="P39" s="12"/>
       <c r="Q39" s="5"/>
       <c r="R39" s="5"/>
     </row>
@@ -2173,49 +2189,49 @@
       <c r="A40" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B40" s="15" t="s">
+      <c r="B40" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="C40" s="15" t="s">
+      <c r="C40" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="D40" s="15" t="s">
+      <c r="D40" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="E40" s="15" t="s">
+      <c r="E40" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="F40" s="15" t="s">
+      <c r="F40" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="G40" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="H40" s="17" t="s">
+      <c r="G40" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="H40" s="11" t="s">
         <v>33</v>
       </c>
       <c r="K40" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L40" s="15" t="s">
+      <c r="L40" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="M40" s="15" t="s">
+      <c r="M40" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="N40" s="15" t="s">
+      <c r="N40" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="O40" s="15" t="s">
+      <c r="O40" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="P40" s="15" t="s">
+      <c r="P40" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="Q40" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="R40" s="17" t="s">
+      <c r="Q40" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="R40" s="11" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2223,23 +2239,23 @@
       <c r="A41" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B41" s="15"/>
-      <c r="C41" s="15"/>
-      <c r="D41" s="15"/>
-      <c r="E41" s="15"/>
-      <c r="F41" s="15"/>
-      <c r="G41" s="17"/>
-      <c r="H41" s="17"/>
+      <c r="B41" s="14"/>
+      <c r="C41" s="14"/>
+      <c r="D41" s="14"/>
+      <c r="E41" s="14"/>
+      <c r="F41" s="14"/>
+      <c r="G41" s="11"/>
+      <c r="H41" s="11"/>
       <c r="K41" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="L41" s="15"/>
-      <c r="M41" s="15"/>
-      <c r="N41" s="15"/>
-      <c r="O41" s="15"/>
-      <c r="P41" s="15"/>
-      <c r="Q41" s="17"/>
-      <c r="R41" s="17"/>
+      <c r="L41" s="14"/>
+      <c r="M41" s="14"/>
+      <c r="N41" s="14"/>
+      <c r="O41" s="14"/>
+      <c r="P41" s="14"/>
+      <c r="Q41" s="11"/>
+      <c r="R41" s="11"/>
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
@@ -2248,40 +2264,40 @@
       <c r="B42" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C42" s="15" t="s">
+      <c r="C42" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="D42" s="15" t="s">
+      <c r="D42" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="E42" s="15" t="s">
+      <c r="E42" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="F42" s="15" t="s">
+      <c r="F42" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="G42" s="17"/>
-      <c r="H42" s="17"/>
+      <c r="G42" s="11"/>
+      <c r="H42" s="11"/>
       <c r="K42" s="3" t="s">
         <v>22</v>
       </c>
       <c r="L42" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="M42" s="15" t="s">
+      <c r="M42" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="N42" s="15" t="s">
+      <c r="N42" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="O42" s="15" t="s">
+      <c r="O42" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="P42" s="15" t="s">
+      <c r="P42" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="Q42" s="17"/>
-      <c r="R42" s="17"/>
+      <c r="Q42" s="11"/>
+      <c r="R42" s="11"/>
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
@@ -2290,24 +2306,24 @@
       <c r="B43" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C43" s="15"/>
-      <c r="D43" s="15"/>
-      <c r="E43" s="15"/>
-      <c r="F43" s="15"/>
-      <c r="G43" s="17"/>
-      <c r="H43" s="17"/>
+      <c r="C43" s="14"/>
+      <c r="D43" s="14"/>
+      <c r="E43" s="14"/>
+      <c r="F43" s="14"/>
+      <c r="G43" s="11"/>
+      <c r="H43" s="11"/>
       <c r="K43" s="3" t="s">
         <v>21</v>
       </c>
       <c r="L43" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="M43" s="15"/>
-      <c r="N43" s="15"/>
-      <c r="O43" s="15"/>
-      <c r="P43" s="15"/>
-      <c r="Q43" s="17"/>
-      <c r="R43" s="17"/>
+      <c r="M43" s="14"/>
+      <c r="N43" s="14"/>
+      <c r="O43" s="14"/>
+      <c r="P43" s="14"/>
+      <c r="Q43" s="11"/>
+      <c r="R43" s="11"/>
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
@@ -2363,49 +2379,49 @@
       <c r="A45" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B45" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="C45" s="17" t="s">
+      <c r="B45" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C45" s="11" t="s">
         <v>33</v>
       </c>
       <c r="D45" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="E45" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="F45" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="G45" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="H45" s="22" t="s">
+      <c r="E45" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F45" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="G45" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="H45" s="18" t="s">
         <v>33</v>
       </c>
       <c r="K45" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="L45" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="M45" s="17" t="s">
+      <c r="L45" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="M45" s="11" t="s">
         <v>33</v>
       </c>
       <c r="N45" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="O45" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="P45" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q45" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="R45" s="22" t="s">
+      <c r="O45" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="P45" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q45" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="R45" s="18" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2413,111 +2429,111 @@
       <c r="A46" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B46" s="17"/>
-      <c r="C46" s="17"/>
-      <c r="D46" s="15" t="s">
+      <c r="B46" s="11"/>
+      <c r="C46" s="11"/>
+      <c r="D46" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="E46" s="17"/>
-      <c r="F46" s="17"/>
-      <c r="G46" s="23"/>
-      <c r="H46" s="23"/>
+      <c r="E46" s="11"/>
+      <c r="F46" s="11"/>
+      <c r="G46" s="19"/>
+      <c r="H46" s="19"/>
       <c r="K46" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="L46" s="17"/>
-      <c r="M46" s="17"/>
-      <c r="N46" s="15" t="s">
+      <c r="L46" s="11"/>
+      <c r="M46" s="11"/>
+      <c r="N46" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="O46" s="17"/>
-      <c r="P46" s="17"/>
-      <c r="Q46" s="23"/>
-      <c r="R46" s="23"/>
+      <c r="O46" s="11"/>
+      <c r="P46" s="11"/>
+      <c r="Q46" s="19"/>
+      <c r="R46" s="19"/>
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B47" s="15" t="s">
+      <c r="B47" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="C47" s="15" t="s">
+      <c r="C47" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="D47" s="15"/>
-      <c r="E47" s="17"/>
-      <c r="F47" s="15" t="s">
+      <c r="D47" s="14"/>
+      <c r="E47" s="11"/>
+      <c r="F47" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="G47" s="23"/>
-      <c r="H47" s="23"/>
+      <c r="G47" s="19"/>
+      <c r="H47" s="19"/>
       <c r="K47" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="L47" s="15" t="s">
+      <c r="L47" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="M47" s="15" t="s">
+      <c r="M47" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="N47" s="15"/>
-      <c r="O47" s="17"/>
-      <c r="P47" s="15" t="s">
+      <c r="N47" s="14"/>
+      <c r="O47" s="11"/>
+      <c r="P47" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="Q47" s="23"/>
-      <c r="R47" s="23"/>
+      <c r="Q47" s="19"/>
+      <c r="R47" s="19"/>
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B48" s="15"/>
-      <c r="C48" s="15"/>
-      <c r="D48" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="E48" s="17"/>
-      <c r="F48" s="15"/>
-      <c r="G48" s="23"/>
-      <c r="H48" s="24"/>
+      <c r="B48" s="14"/>
+      <c r="C48" s="14"/>
+      <c r="D48" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E48" s="11"/>
+      <c r="F48" s="14"/>
+      <c r="G48" s="19"/>
+      <c r="H48" s="20"/>
       <c r="K48" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="L48" s="15"/>
-      <c r="M48" s="15"/>
-      <c r="N48" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="O48" s="17"/>
-      <c r="P48" s="15"/>
-      <c r="Q48" s="23"/>
-      <c r="R48" s="24"/>
+      <c r="L48" s="14"/>
+      <c r="M48" s="14"/>
+      <c r="N48" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="O48" s="11"/>
+      <c r="P48" s="14"/>
+      <c r="Q48" s="19"/>
+      <c r="R48" s="20"/>
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B49" s="15"/>
-      <c r="C49" s="15"/>
-      <c r="D49" s="17"/>
-      <c r="E49" s="17"/>
-      <c r="F49" s="15"/>
-      <c r="G49" s="24"/>
-      <c r="H49" s="25" t="s">
+      <c r="B49" s="14"/>
+      <c r="C49" s="14"/>
+      <c r="D49" s="11"/>
+      <c r="E49" s="11"/>
+      <c r="F49" s="14"/>
+      <c r="G49" s="20"/>
+      <c r="H49" s="21" t="s">
         <v>53</v>
       </c>
       <c r="K49" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="L49" s="15"/>
-      <c r="M49" s="15"/>
-      <c r="N49" s="17"/>
-      <c r="O49" s="17"/>
-      <c r="P49" s="15"/>
-      <c r="Q49" s="24"/>
-      <c r="R49" s="25" t="s">
+      <c r="L49" s="14"/>
+      <c r="M49" s="14"/>
+      <c r="N49" s="11"/>
+      <c r="O49" s="11"/>
+      <c r="P49" s="14"/>
+      <c r="Q49" s="20"/>
+      <c r="R49" s="21" t="s">
         <v>53</v>
       </c>
     </row>
@@ -2525,57 +2541,57 @@
       <c r="A50" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B50" s="16" t="s">
+      <c r="B50" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="C50" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="D50" s="16" t="s">
+      <c r="C50" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D50" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="E50" s="15" t="s">
+      <c r="E50" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="F50" s="16" t="s">
+      <c r="F50" s="13" t="s">
         <v>43</v>
       </c>
       <c r="G50" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="H50" s="26"/>
+      <c r="H50" s="22"/>
       <c r="K50" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="L50" s="16" t="s">
+      <c r="L50" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="M50" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="N50" s="16" t="s">
+      <c r="M50" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="N50" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="O50" s="15" t="s">
+      <c r="O50" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="P50" s="16" t="s">
+      <c r="P50" s="13" t="s">
         <v>43</v>
       </c>
       <c r="Q50" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="R50" s="26"/>
+      <c r="R50" s="22"/>
     </row>
     <row r="51" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B51" s="16"/>
-      <c r="C51" s="18"/>
-      <c r="D51" s="16"/>
-      <c r="E51" s="15"/>
-      <c r="F51" s="16"/>
+      <c r="B51" s="13"/>
+      <c r="C51" s="12"/>
+      <c r="D51" s="13"/>
+      <c r="E51" s="14"/>
+      <c r="F51" s="13"/>
       <c r="G51" s="8" t="s">
         <v>36</v>
       </c>
@@ -2585,11 +2601,11 @@
       <c r="K51" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="L51" s="16"/>
-      <c r="M51" s="18"/>
-      <c r="N51" s="16"/>
-      <c r="O51" s="15"/>
-      <c r="P51" s="16"/>
+      <c r="L51" s="13"/>
+      <c r="M51" s="12"/>
+      <c r="N51" s="13"/>
+      <c r="O51" s="14"/>
+      <c r="P51" s="13"/>
       <c r="Q51" s="8" t="s">
         <v>81</v>
       </c>
@@ -2610,14 +2626,14 @@
       <c r="D52" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="E52" s="15"/>
+      <c r="E52" s="14"/>
       <c r="F52" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="G52" s="21" t="s">
+      <c r="G52" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="H52" s="11" t="s">
+      <c r="H52" s="27" t="s">
         <v>49</v>
       </c>
       <c r="K52" s="2" t="s">
@@ -2632,14 +2648,14 @@
       <c r="N52" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="O52" s="15"/>
+      <c r="O52" s="14"/>
       <c r="P52" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="Q52" s="21" t="s">
+      <c r="Q52" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="R52" s="19" t="s">
+      <c r="R52" s="16" t="s">
         <v>49</v>
       </c>
     </row>
@@ -2647,13 +2663,13 @@
       <c r="A53" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B53" s="19" t="s">
+      <c r="B53" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="C53" s="19" t="s">
+      <c r="C53" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="D53" s="19" t="s">
+      <c r="D53" s="16" t="s">
         <v>49</v>
       </c>
       <c r="E53" s="8" t="s">
@@ -2662,18 +2678,18 @@
       <c r="F53" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="G53" s="21"/>
-      <c r="H53" s="12"/>
+      <c r="G53" s="15"/>
+      <c r="H53" s="28"/>
       <c r="K53" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="L53" s="19" t="s">
+      <c r="L53" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="M53" s="19" t="s">
+      <c r="M53" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="N53" s="19" t="s">
+      <c r="N53" s="16" t="s">
         <v>49</v>
       </c>
       <c r="O53" s="8" t="s">
@@ -2682,42 +2698,42 @@
       <c r="P53" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="Q53" s="21"/>
-      <c r="R53" s="19"/>
+      <c r="Q53" s="15"/>
+      <c r="R53" s="16"/>
     </row>
     <row r="54" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B54" s="19"/>
-      <c r="C54" s="19"/>
-      <c r="D54" s="19"/>
+      <c r="B54" s="16"/>
+      <c r="C54" s="16"/>
+      <c r="D54" s="16"/>
       <c r="E54" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="F54" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="G54" s="20" t="s">
+      <c r="F54" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="G54" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="H54" s="13"/>
+      <c r="H54" s="29"/>
       <c r="K54" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="L54" s="19"/>
-      <c r="M54" s="19"/>
-      <c r="N54" s="19"/>
+      <c r="L54" s="16"/>
+      <c r="M54" s="16"/>
+      <c r="N54" s="16"/>
       <c r="O54" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="P54" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q54" s="20" t="s">
+      <c r="P54" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q54" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="R54" s="19"/>
+      <c r="R54" s="16"/>
     </row>
     <row r="55" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
@@ -2735,8 +2751,8 @@
       <c r="E55" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="F55" s="20"/>
-      <c r="G55" s="20"/>
+      <c r="F55" s="17"/>
+      <c r="G55" s="17"/>
       <c r="H55" s="10" t="s">
         <v>32</v>
       </c>
@@ -2755,25 +2771,168 @@
       <c r="O55" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="P55" s="20"/>
-      <c r="Q55" s="20"/>
+      <c r="P55" s="17"/>
+      <c r="Q55" s="17"/>
       <c r="R55" s="10" t="s">
         <v>32</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="190">
-    <mergeCell ref="M50:M51"/>
-    <mergeCell ref="N50:N51"/>
-    <mergeCell ref="O50:O52"/>
-    <mergeCell ref="P50:P51"/>
-    <mergeCell ref="Q52:Q53"/>
-    <mergeCell ref="R52:R54"/>
-    <mergeCell ref="L53:L54"/>
-    <mergeCell ref="M53:M54"/>
-    <mergeCell ref="N53:N54"/>
-    <mergeCell ref="P54:P55"/>
-    <mergeCell ref="Q54:Q55"/>
+  <mergeCells count="189">
+    <mergeCell ref="H45:H48"/>
+    <mergeCell ref="H49:H50"/>
+    <mergeCell ref="G18:G21"/>
+    <mergeCell ref="N19:N22"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="H52:H54"/>
+    <mergeCell ref="C3:C7"/>
+    <mergeCell ref="D3:D7"/>
+    <mergeCell ref="E3:E7"/>
+    <mergeCell ref="F3:F7"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="F25:F26"/>
+    <mergeCell ref="H32:H38"/>
+    <mergeCell ref="G32:G38"/>
+    <mergeCell ref="H40:H43"/>
+    <mergeCell ref="C42:C43"/>
+    <mergeCell ref="D42:D43"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="B3:B7"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E16:E20"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="G23:G24"/>
+    <mergeCell ref="G25:G26"/>
+    <mergeCell ref="H23:H25"/>
+    <mergeCell ref="L3:L7"/>
+    <mergeCell ref="L9:L10"/>
+    <mergeCell ref="L11:L12"/>
+    <mergeCell ref="L16:L17"/>
+    <mergeCell ref="L18:L20"/>
+    <mergeCell ref="F16:F17"/>
+    <mergeCell ref="H16:H19"/>
+    <mergeCell ref="H20:H21"/>
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="G10:G11"/>
+    <mergeCell ref="G3:G8"/>
+    <mergeCell ref="H3:H8"/>
+    <mergeCell ref="H10:H14"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="C18:C20"/>
+    <mergeCell ref="F18:F20"/>
+    <mergeCell ref="E21:E23"/>
+    <mergeCell ref="M3:M7"/>
+    <mergeCell ref="N3:N7"/>
+    <mergeCell ref="O3:O7"/>
+    <mergeCell ref="P3:P7"/>
+    <mergeCell ref="Q3:Q9"/>
+    <mergeCell ref="R3:R9"/>
+    <mergeCell ref="M9:M10"/>
+    <mergeCell ref="N9:N10"/>
+    <mergeCell ref="O9:O10"/>
+    <mergeCell ref="P9:P10"/>
+    <mergeCell ref="M11:M12"/>
+    <mergeCell ref="N11:N12"/>
+    <mergeCell ref="O11:O12"/>
+    <mergeCell ref="P11:P12"/>
+    <mergeCell ref="Q11:Q14"/>
+    <mergeCell ref="R11:R14"/>
+    <mergeCell ref="M13:M14"/>
+    <mergeCell ref="N13:N14"/>
+    <mergeCell ref="O13:O14"/>
+    <mergeCell ref="P13:P14"/>
+    <mergeCell ref="Q16:Q20"/>
+    <mergeCell ref="R16:R19"/>
+    <mergeCell ref="R20:R21"/>
+    <mergeCell ref="M16:M17"/>
+    <mergeCell ref="O16:O20"/>
+    <mergeCell ref="P16:P17"/>
+    <mergeCell ref="N17:N18"/>
+    <mergeCell ref="M18:M20"/>
+    <mergeCell ref="P18:P20"/>
+    <mergeCell ref="R23:R25"/>
+    <mergeCell ref="L24:L25"/>
+    <mergeCell ref="M24:M25"/>
+    <mergeCell ref="N24:N25"/>
+    <mergeCell ref="P25:P26"/>
+    <mergeCell ref="Q25:Q26"/>
+    <mergeCell ref="L21:L22"/>
+    <mergeCell ref="M21:M22"/>
+    <mergeCell ref="O21:O23"/>
+    <mergeCell ref="P21:P22"/>
+    <mergeCell ref="Q23:Q24"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="C38:C39"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="E38:E39"/>
+    <mergeCell ref="F38:F39"/>
+    <mergeCell ref="B32:B36"/>
+    <mergeCell ref="C32:C36"/>
+    <mergeCell ref="D32:D36"/>
+    <mergeCell ref="E32:E36"/>
+    <mergeCell ref="F32:F36"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="C45:C46"/>
+    <mergeCell ref="E45:E49"/>
+    <mergeCell ref="F45:F46"/>
+    <mergeCell ref="G45:G49"/>
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="C40:C41"/>
+    <mergeCell ref="D40:D41"/>
+    <mergeCell ref="E40:E41"/>
+    <mergeCell ref="F40:F41"/>
+    <mergeCell ref="G40:G43"/>
+    <mergeCell ref="D46:D47"/>
+    <mergeCell ref="B47:B49"/>
+    <mergeCell ref="C47:C49"/>
+    <mergeCell ref="F47:F49"/>
+    <mergeCell ref="D48:D49"/>
+    <mergeCell ref="E42:E43"/>
+    <mergeCell ref="F42:F43"/>
+    <mergeCell ref="B50:B51"/>
+    <mergeCell ref="C50:C51"/>
+    <mergeCell ref="D50:D51"/>
+    <mergeCell ref="E50:E52"/>
+    <mergeCell ref="F50:F51"/>
+    <mergeCell ref="G52:G53"/>
+    <mergeCell ref="B53:B54"/>
+    <mergeCell ref="C53:C54"/>
+    <mergeCell ref="D53:D54"/>
+    <mergeCell ref="F54:F55"/>
+    <mergeCell ref="G54:G55"/>
+    <mergeCell ref="R32:R38"/>
+    <mergeCell ref="L38:L39"/>
+    <mergeCell ref="M38:M39"/>
+    <mergeCell ref="N38:N39"/>
+    <mergeCell ref="O38:O39"/>
+    <mergeCell ref="P38:P39"/>
+    <mergeCell ref="L32:L36"/>
+    <mergeCell ref="M32:M36"/>
+    <mergeCell ref="N32:N36"/>
+    <mergeCell ref="O32:O36"/>
+    <mergeCell ref="P32:P36"/>
+    <mergeCell ref="Q32:Q38"/>
     <mergeCell ref="R40:R43"/>
     <mergeCell ref="M42:M43"/>
     <mergeCell ref="N42:N43"/>
@@ -2798,161 +2957,17 @@
     <mergeCell ref="N48:N49"/>
     <mergeCell ref="R49:R50"/>
     <mergeCell ref="L50:L51"/>
-    <mergeCell ref="R32:R38"/>
-    <mergeCell ref="L38:L39"/>
-    <mergeCell ref="M38:M39"/>
-    <mergeCell ref="N38:N39"/>
-    <mergeCell ref="O38:O39"/>
-    <mergeCell ref="P38:P39"/>
-    <mergeCell ref="L32:L36"/>
-    <mergeCell ref="M32:M36"/>
-    <mergeCell ref="N32:N36"/>
-    <mergeCell ref="O32:O36"/>
-    <mergeCell ref="P32:P36"/>
-    <mergeCell ref="Q32:Q38"/>
-    <mergeCell ref="B50:B51"/>
-    <mergeCell ref="C50:C51"/>
-    <mergeCell ref="D50:D51"/>
-    <mergeCell ref="E50:E52"/>
-    <mergeCell ref="F50:F51"/>
-    <mergeCell ref="G52:G53"/>
-    <mergeCell ref="B53:B54"/>
-    <mergeCell ref="C53:C54"/>
-    <mergeCell ref="D53:D54"/>
-    <mergeCell ref="F54:F55"/>
-    <mergeCell ref="G54:G55"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="C45:C46"/>
-    <mergeCell ref="E45:E49"/>
-    <mergeCell ref="F45:F46"/>
-    <mergeCell ref="G45:G49"/>
-    <mergeCell ref="B40:B41"/>
-    <mergeCell ref="C40:C41"/>
-    <mergeCell ref="D40:D41"/>
-    <mergeCell ref="E40:E41"/>
-    <mergeCell ref="F40:F41"/>
-    <mergeCell ref="G40:G43"/>
-    <mergeCell ref="D46:D47"/>
-    <mergeCell ref="B47:B49"/>
-    <mergeCell ref="C47:C49"/>
-    <mergeCell ref="F47:F49"/>
-    <mergeCell ref="D48:D49"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="C38:C39"/>
-    <mergeCell ref="D38:D39"/>
-    <mergeCell ref="E38:E39"/>
-    <mergeCell ref="F38:F39"/>
-    <mergeCell ref="B32:B36"/>
-    <mergeCell ref="C32:C36"/>
-    <mergeCell ref="D32:D36"/>
-    <mergeCell ref="E32:E36"/>
-    <mergeCell ref="F32:F36"/>
-    <mergeCell ref="R23:R25"/>
-    <mergeCell ref="L24:L25"/>
-    <mergeCell ref="M24:M25"/>
-    <mergeCell ref="N24:N25"/>
-    <mergeCell ref="P25:P26"/>
-    <mergeCell ref="Q25:Q26"/>
-    <mergeCell ref="L21:L22"/>
-    <mergeCell ref="M21:M22"/>
-    <mergeCell ref="N21:N22"/>
-    <mergeCell ref="O21:O23"/>
-    <mergeCell ref="P21:P22"/>
-    <mergeCell ref="Q23:Q24"/>
-    <mergeCell ref="N19:N20"/>
-    <mergeCell ref="M11:M12"/>
-    <mergeCell ref="N11:N12"/>
-    <mergeCell ref="O11:O12"/>
-    <mergeCell ref="P11:P12"/>
-    <mergeCell ref="Q11:Q14"/>
-    <mergeCell ref="R11:R14"/>
-    <mergeCell ref="M13:M14"/>
-    <mergeCell ref="N13:N14"/>
-    <mergeCell ref="O13:O14"/>
-    <mergeCell ref="P13:P14"/>
-    <mergeCell ref="Q16:Q20"/>
-    <mergeCell ref="R16:R19"/>
-    <mergeCell ref="R20:R21"/>
-    <mergeCell ref="M16:M17"/>
-    <mergeCell ref="O16:O20"/>
-    <mergeCell ref="P16:P17"/>
-    <mergeCell ref="N17:N18"/>
-    <mergeCell ref="M18:M20"/>
-    <mergeCell ref="P18:P20"/>
-    <mergeCell ref="M3:M7"/>
-    <mergeCell ref="N3:N7"/>
-    <mergeCell ref="O3:O7"/>
-    <mergeCell ref="P3:P7"/>
-    <mergeCell ref="Q3:Q9"/>
-    <mergeCell ref="R3:R9"/>
-    <mergeCell ref="M9:M10"/>
-    <mergeCell ref="N9:N10"/>
-    <mergeCell ref="O9:O10"/>
-    <mergeCell ref="P9:P10"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="G23:G24"/>
-    <mergeCell ref="G25:G26"/>
-    <mergeCell ref="H23:H25"/>
-    <mergeCell ref="L3:L7"/>
-    <mergeCell ref="L9:L10"/>
-    <mergeCell ref="L11:L12"/>
-    <mergeCell ref="L16:L17"/>
-    <mergeCell ref="L18:L20"/>
-    <mergeCell ref="F16:F17"/>
-    <mergeCell ref="H16:H19"/>
-    <mergeCell ref="H20:H21"/>
-    <mergeCell ref="G12:G13"/>
-    <mergeCell ref="G10:G11"/>
-    <mergeCell ref="G3:G8"/>
-    <mergeCell ref="H3:H8"/>
-    <mergeCell ref="H10:H14"/>
-    <mergeCell ref="G16:G17"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="F21:F22"/>
-    <mergeCell ref="C18:C20"/>
-    <mergeCell ref="F18:F20"/>
-    <mergeCell ref="E21:E23"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="B3:B7"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="E16:E20"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="H52:H54"/>
-    <mergeCell ref="C3:C7"/>
-    <mergeCell ref="D3:D7"/>
-    <mergeCell ref="E3:E7"/>
-    <mergeCell ref="F3:F7"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="F25:F26"/>
-    <mergeCell ref="H32:H38"/>
-    <mergeCell ref="G32:G38"/>
-    <mergeCell ref="H40:H43"/>
-    <mergeCell ref="C42:C43"/>
-    <mergeCell ref="D42:D43"/>
-    <mergeCell ref="E42:E43"/>
-    <mergeCell ref="F42:F43"/>
-    <mergeCell ref="H45:H48"/>
-    <mergeCell ref="H49:H50"/>
-    <mergeCell ref="G18:G21"/>
+    <mergeCell ref="M50:M51"/>
+    <mergeCell ref="N50:N51"/>
+    <mergeCell ref="O50:O52"/>
+    <mergeCell ref="P50:P51"/>
+    <mergeCell ref="Q52:Q53"/>
+    <mergeCell ref="R52:R54"/>
+    <mergeCell ref="L53:L54"/>
+    <mergeCell ref="M53:M54"/>
+    <mergeCell ref="N53:N54"/>
+    <mergeCell ref="P54:P55"/>
+    <mergeCell ref="Q54:Q55"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>